<commit_message>
laid groundwork for changing error colors
</commit_message>
<xml_diff>
--- a/app/spreadsheets/sample.xlsx
+++ b/app/spreadsheets/sample.xlsx
@@ -514,7 +514,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
@@ -6506,7 +6506,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added error handling for color selector and function buttons
</commit_message>
<xml_diff>
--- a/app/spreadsheets/sample.xlsx
+++ b/app/spreadsheets/sample.xlsx
@@ -57,7 +57,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -82,6 +82,24 @@
         <bgColor rgb="FFEFBE7D"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF787FFF"/>
+        <bgColor rgb="FF787FFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF545FFF"/>
+        <bgColor rgb="FF545FFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE79DFF"/>
+        <bgColor rgb="FFE79DFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -95,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -237,6 +255,61 @@
     </xf>
     <xf numFmtId="165" fontId="2" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="3" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,95 +769,95 @@
       <c r="AG1" s="4" t="n"/>
     </row>
     <row r="2" ht="15.75" customHeight="1" s="5">
-      <c r="A2" s="60" t="inlineStr">
+      <c r="A2" s="89" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B2" s="61" t="n">
+      <c r="B2" s="90" t="n">
         <v>13295</v>
       </c>
-      <c r="C2" s="62" t="n"/>
-      <c r="D2" s="62" t="n"/>
-      <c r="E2" s="62" t="n"/>
-      <c r="F2" s="63" t="inlineStr">
+      <c r="C2" s="91" t="n"/>
+      <c r="D2" s="91" t="n"/>
+      <c r="E2" s="91" t="n"/>
+      <c r="F2" s="92" t="inlineStr">
         <is>
           <t>Technical papers and other research articles by William Stanley</t>
         </is>
       </c>
-      <c r="G2" s="62" t="n"/>
-      <c r="H2" s="63" t="inlineStr">
+      <c r="G2" s="91" t="n"/>
+      <c r="H2" s="92" t="inlineStr">
         <is>
           <t xml:space="preserve">Stanley Ferrostat Vaccum Products Pamphlet </t>
         </is>
       </c>
-      <c r="I2" s="62" t="n"/>
-      <c r="J2" s="62" t="n"/>
-      <c r="K2" s="62" t="n"/>
-      <c r="L2" s="62" t="n"/>
-      <c r="M2" s="60" t="inlineStr">
+      <c r="I2" s="91" t="n"/>
+      <c r="J2" s="91" t="n"/>
+      <c r="K2" s="91" t="n"/>
+      <c r="L2" s="91" t="n"/>
+      <c r="M2" s="89" t="inlineStr">
         <is>
           <t>1887 - 1913</t>
         </is>
       </c>
-      <c r="N2" s="62" t="n"/>
-      <c r="O2" s="62" t="n"/>
-      <c r="P2" s="64" t="n">
+      <c r="N2" s="91" t="n"/>
+      <c r="O2" s="91" t="n"/>
+      <c r="P2" s="93" t="n">
         <v>1913</v>
       </c>
-      <c r="Q2" s="62" t="n"/>
-      <c r="R2" s="63" t="inlineStr">
+      <c r="Q2" s="91" t="n"/>
+      <c r="R2" s="92" t="inlineStr">
         <is>
           <t xml:space="preserve">No Copyright - United States </t>
         </is>
       </c>
-      <c r="S2" s="62" t="inlineStr">
+      <c r="S2" s="91" t="inlineStr">
         <is>
           <t xml:space="preserve">2 pages </t>
         </is>
       </c>
-      <c r="T2" s="62" t="inlineStr">
+      <c r="T2" s="91" t="inlineStr">
         <is>
           <t xml:space="preserve">Box 8, Folder 1, Item 1 </t>
         </is>
       </c>
-      <c r="U2" s="62" t="inlineStr">
+      <c r="U2" s="91" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down. </t>
         </is>
       </c>
-      <c r="V2" s="62" t="n">
+      <c r="V2" s="91" t="n">
         <v>0</v>
       </c>
-      <c r="W2" s="65" t="n">
+      <c r="W2" s="94" t="n">
         <v>45506</v>
       </c>
-      <c r="X2" s="62" t="inlineStr">
+      <c r="X2" s="91" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
-      <c r="Y2" s="62" t="n"/>
-      <c r="Z2" s="66" t="inlineStr">
+      <c r="Y2" s="91" t="n"/>
+      <c r="Z2" s="95" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA2" s="62" t="inlineStr">
+      <c r="AA2" s="91" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB2" s="62" t="inlineStr">
+      <c r="AB2" s="91" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC2" s="62" t="n"/>
-      <c r="AD2" s="62" t="n"/>
-      <c r="AE2" s="62" t="n"/>
-      <c r="AF2" s="62" t="n"/>
-      <c r="AG2" s="62" t="n"/>
+      <c r="AC2" s="91" t="n"/>
+      <c r="AD2" s="91" t="n"/>
+      <c r="AE2" s="91" t="n"/>
+      <c r="AF2" s="91" t="n"/>
+      <c r="AG2" s="91" t="n"/>
     </row>
     <row r="3" ht="15.75" customHeight="1" s="5">
       <c r="A3" s="1" t="inlineStr">
@@ -1766,935 +1839,935 @@
       <c r="AG13" s="4" t="n"/>
     </row>
     <row r="14" ht="15.75" customHeight="1" s="5">
-      <c r="A14" s="45" t="inlineStr">
+      <c r="A14" s="74" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B14" s="46" t="n">
+      <c r="B14" s="75" t="n">
         <v>13300</v>
       </c>
-      <c r="C14" s="47" t="n"/>
-      <c r="D14" s="47" t="n"/>
-      <c r="E14" s="47" t="n"/>
-      <c r="F14" s="48" t="inlineStr">
+      <c r="C14" s="76" t="n"/>
+      <c r="D14" s="76" t="n"/>
+      <c r="E14" s="76" t="n"/>
+      <c r="F14" s="77" t="inlineStr">
         <is>
           <t>William Stanley biography, early transcript draft with manuscript inserts</t>
         </is>
       </c>
-      <c r="G14" s="47" t="n"/>
-      <c r="H14" s="48" t="inlineStr">
+      <c r="G14" s="76" t="n"/>
+      <c r="H14" s="77" t="inlineStr">
         <is>
           <t>Sections of Typescript Draft of "The Life of William Stanley" by Thomas C. Martin, "Stanley as Inventor and Manufacturer at Pittsfield"</t>
         </is>
       </c>
-      <c r="I14" s="47" t="n"/>
-      <c r="J14" s="45" t="inlineStr">
+      <c r="I14" s="76" t="n"/>
+      <c r="J14" s="74" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="K14" s="45" t="inlineStr">
+      <c r="K14" s="74" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L14" s="47" t="n"/>
-      <c r="M14" s="45" t="inlineStr">
+      <c r="L14" s="76" t="n"/>
+      <c r="M14" s="74" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N14" s="47" t="n"/>
-      <c r="O14" s="47" t="n"/>
-      <c r="P14" s="49" t="inlineStr">
+      <c r="N14" s="76" t="n"/>
+      <c r="O14" s="76" t="n"/>
+      <c r="P14" s="78" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q14" s="47" t="n"/>
-      <c r="R14" s="48" t="inlineStr">
+      <c r="Q14" s="76" t="n"/>
+      <c r="R14" s="77" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S14" s="50" t="inlineStr">
+      <c r="S14" s="79" t="inlineStr">
         <is>
           <t xml:space="preserve">14 pages </t>
         </is>
       </c>
-      <c r="T14" s="47" t="inlineStr">
+      <c r="T14" s="76" t="inlineStr">
         <is>
           <t xml:space="preserve">Box 8, Folder 6, Item 1  </t>
         </is>
       </c>
-      <c r="U14" s="47" t="inlineStr">
+      <c r="U14" s="76" t="inlineStr">
         <is>
           <t>Glass Down. Goes until Page 14. Please make sure you scan complete section.</t>
         </is>
       </c>
-      <c r="V14" s="47" t="inlineStr">
+      <c r="V14" s="76" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F06.01</t>
         </is>
       </c>
-      <c r="W14" s="51" t="n">
+      <c r="W14" s="80" t="n">
         <v>45510</v>
       </c>
-      <c r="X14" s="50" t="inlineStr">
+      <c r="X14" s="79" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y14" s="47" t="n"/>
-      <c r="Z14" s="52" t="inlineStr">
+      <c r="Y14" s="76" t="n"/>
+      <c r="Z14" s="81" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA14" s="47" t="inlineStr">
+      <c r="AA14" s="76" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB14" s="47" t="inlineStr">
+      <c r="AB14" s="76" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC14" s="47" t="n"/>
-      <c r="AD14" s="47" t="n"/>
-      <c r="AE14" s="47" t="n"/>
-      <c r="AF14" s="47" t="n"/>
-      <c r="AG14" s="47" t="n"/>
+      <c r="AC14" s="76" t="n"/>
+      <c r="AD14" s="76" t="n"/>
+      <c r="AE14" s="76" t="n"/>
+      <c r="AF14" s="76" t="n"/>
+      <c r="AG14" s="76" t="n"/>
     </row>
     <row r="15" ht="15.75" customHeight="1" s="5">
-      <c r="A15" s="45" t="inlineStr">
+      <c r="A15" s="74" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B15" s="46" t="n">
+      <c r="B15" s="75" t="n">
         <v>13300</v>
       </c>
-      <c r="C15" s="47" t="n"/>
-      <c r="D15" s="47" t="n"/>
-      <c r="E15" s="47" t="n"/>
-      <c r="F15" s="48" t="inlineStr">
+      <c r="C15" s="76" t="n"/>
+      <c r="D15" s="76" t="n"/>
+      <c r="E15" s="76" t="n"/>
+      <c r="F15" s="77" t="inlineStr">
         <is>
           <t>William Stanley biography, early transcript draft with manuscript inserts</t>
         </is>
       </c>
-      <c r="G15" s="47" t="n"/>
-      <c r="H15" s="48" t="inlineStr">
+      <c r="G15" s="76" t="n"/>
+      <c r="H15" s="77" t="inlineStr">
         <is>
           <t xml:space="preserve">Sections of Typescript Draft of "The Life of William Stanley" by Thomas C. Martin, Untitiled from Scientific and Industrial Information Bureau </t>
         </is>
       </c>
-      <c r="I15" s="47" t="n"/>
-      <c r="J15" s="45" t="inlineStr">
+      <c r="I15" s="76" t="n"/>
+      <c r="J15" s="74" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="K15" s="45" t="inlineStr">
+      <c r="K15" s="74" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L15" s="47" t="n"/>
-      <c r="M15" s="45" t="inlineStr">
+      <c r="L15" s="76" t="n"/>
+      <c r="M15" s="74" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N15" s="47" t="n"/>
-      <c r="O15" s="47" t="n"/>
-      <c r="P15" s="49" t="inlineStr">
+      <c r="N15" s="76" t="n"/>
+      <c r="O15" s="76" t="n"/>
+      <c r="P15" s="78" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q15" s="47" t="n"/>
-      <c r="R15" s="48" t="inlineStr">
+      <c r="Q15" s="76" t="n"/>
+      <c r="R15" s="77" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S15" s="50" t="inlineStr">
+      <c r="S15" s="79" t="inlineStr">
         <is>
           <t xml:space="preserve">21 pages </t>
         </is>
       </c>
-      <c r="T15" s="47" t="inlineStr">
+      <c r="T15" s="76" t="inlineStr">
         <is>
           <t>Box 8, Folder 6, Item 2</t>
         </is>
       </c>
-      <c r="U15" s="47" t="inlineStr">
+      <c r="U15" s="76" t="inlineStr">
         <is>
           <t>Glass Down. Use white paper as marker for section. Please make sure you scan complete section.</t>
         </is>
       </c>
-      <c r="V15" s="47" t="inlineStr">
+      <c r="V15" s="76" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F06.02</t>
         </is>
       </c>
-      <c r="W15" s="51" t="n">
+      <c r="W15" s="80" t="n">
         <v>45511</v>
       </c>
-      <c r="X15" s="50" t="inlineStr">
+      <c r="X15" s="79" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y15" s="47" t="n"/>
-      <c r="Z15" s="52" t="inlineStr">
+      <c r="Y15" s="76" t="n"/>
+      <c r="Z15" s="81" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA15" s="47" t="inlineStr">
+      <c r="AA15" s="76" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB15" s="47" t="inlineStr">
+      <c r="AB15" s="76" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC15" s="47" t="n"/>
-      <c r="AD15" s="47" t="n"/>
-      <c r="AE15" s="47" t="n"/>
-      <c r="AF15" s="47" t="n"/>
-      <c r="AG15" s="47" t="n"/>
+      <c r="AC15" s="76" t="n"/>
+      <c r="AD15" s="76" t="n"/>
+      <c r="AE15" s="76" t="n"/>
+      <c r="AF15" s="76" t="n"/>
+      <c r="AG15" s="76" t="n"/>
     </row>
     <row r="16" ht="15.75" customHeight="1" s="5">
-      <c r="A16" s="45" t="inlineStr">
+      <c r="A16" s="74" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B16" s="46" t="n">
+      <c r="B16" s="75" t="n">
         <v>13300</v>
       </c>
-      <c r="C16" s="47" t="n"/>
-      <c r="D16" s="47" t="n"/>
-      <c r="E16" s="47" t="n"/>
-      <c r="F16" s="48" t="inlineStr">
+      <c r="C16" s="76" t="n"/>
+      <c r="D16" s="76" t="n"/>
+      <c r="E16" s="76" t="n"/>
+      <c r="F16" s="77" t="inlineStr">
         <is>
           <t>William Stanley biography, early transcript draft with manuscript inserts</t>
         </is>
       </c>
-      <c r="G16" s="47" t="n"/>
-      <c r="H16" s="48" t="inlineStr">
+      <c r="G16" s="76" t="n"/>
+      <c r="H16" s="77" t="inlineStr">
         <is>
           <t xml:space="preserve">Sections of Typescript Draft of "The Life of William Stanley" by Thomas C. Martin, Untitiled </t>
         </is>
       </c>
-      <c r="I16" s="47" t="n"/>
-      <c r="J16" s="45" t="inlineStr">
+      <c r="I16" s="76" t="n"/>
+      <c r="J16" s="74" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="K16" s="45" t="inlineStr">
+      <c r="K16" s="74" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L16" s="47" t="n"/>
-      <c r="M16" s="45" t="inlineStr">
+      <c r="L16" s="76" t="n"/>
+      <c r="M16" s="74" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N16" s="47" t="n"/>
-      <c r="O16" s="47" t="n"/>
-      <c r="P16" s="49" t="inlineStr">
+      <c r="N16" s="76" t="n"/>
+      <c r="O16" s="76" t="n"/>
+      <c r="P16" s="78" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q16" s="47" t="n"/>
-      <c r="R16" s="48" t="inlineStr">
+      <c r="Q16" s="76" t="n"/>
+      <c r="R16" s="77" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S16" s="50" t="inlineStr">
+      <c r="S16" s="79" t="inlineStr">
         <is>
           <t xml:space="preserve">5 pages </t>
         </is>
       </c>
-      <c r="T16" s="47" t="inlineStr">
+      <c r="T16" s="76" t="inlineStr">
         <is>
           <t>Box 8, Folder 6, Item 3</t>
         </is>
       </c>
-      <c r="U16" s="47" t="inlineStr">
+      <c r="U16" s="76" t="inlineStr">
         <is>
           <t>Glass Up. Use white paper as marker for section. Please make sure you scan complete section.</t>
         </is>
       </c>
-      <c r="V16" s="47" t="inlineStr">
+      <c r="V16" s="76" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F06.03</t>
         </is>
       </c>
-      <c r="W16" s="51" t="n">
+      <c r="W16" s="80" t="n">
         <v>45511</v>
       </c>
-      <c r="X16" s="50" t="inlineStr">
+      <c r="X16" s="79" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y16" s="47" t="n"/>
-      <c r="Z16" s="52" t="inlineStr">
+      <c r="Y16" s="76" t="n"/>
+      <c r="Z16" s="81" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA16" s="47" t="inlineStr">
+      <c r="AA16" s="76" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB16" s="47" t="inlineStr">
+      <c r="AB16" s="76" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC16" s="47" t="n"/>
-      <c r="AD16" s="47" t="n"/>
-      <c r="AE16" s="47" t="n"/>
-      <c r="AF16" s="47" t="n"/>
-      <c r="AG16" s="47" t="n"/>
+      <c r="AC16" s="76" t="n"/>
+      <c r="AD16" s="76" t="n"/>
+      <c r="AE16" s="76" t="n"/>
+      <c r="AF16" s="76" t="n"/>
+      <c r="AG16" s="76" t="n"/>
     </row>
     <row r="17" ht="15.75" customHeight="1" s="5">
-      <c r="A17" s="45" t="inlineStr">
+      <c r="A17" s="74" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B17" s="46" t="n">
+      <c r="B17" s="75" t="n">
         <v>13300</v>
       </c>
-      <c r="C17" s="47" t="n"/>
-      <c r="D17" s="47" t="n"/>
-      <c r="E17" s="47" t="n"/>
-      <c r="F17" s="48" t="inlineStr">
+      <c r="C17" s="76" t="n"/>
+      <c r="D17" s="76" t="n"/>
+      <c r="E17" s="76" t="n"/>
+      <c r="F17" s="77" t="inlineStr">
         <is>
           <t>William Stanley biography, early transcript draft with manuscript inserts</t>
         </is>
       </c>
-      <c r="G17" s="47" t="n"/>
-      <c r="H17" s="48" t="inlineStr">
+      <c r="G17" s="76" t="n"/>
+      <c r="H17" s="77" t="inlineStr">
         <is>
           <t>Author's Notes on "The Life of William Stanley" Trnascript by Thomas C. Martin</t>
         </is>
       </c>
-      <c r="I17" s="47" t="n"/>
-      <c r="J17" s="45" t="inlineStr">
+      <c r="I17" s="76" t="n"/>
+      <c r="J17" s="74" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="K17" s="45" t="inlineStr">
+      <c r="K17" s="74" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L17" s="47" t="n"/>
-      <c r="M17" s="45" t="inlineStr">
+      <c r="L17" s="76" t="n"/>
+      <c r="M17" s="74" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N17" s="47" t="n"/>
-      <c r="O17" s="47" t="n"/>
-      <c r="P17" s="49" t="inlineStr">
+      <c r="N17" s="76" t="n"/>
+      <c r="O17" s="76" t="n"/>
+      <c r="P17" s="78" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q17" s="47" t="n"/>
-      <c r="R17" s="48" t="inlineStr">
+      <c r="Q17" s="76" t="n"/>
+      <c r="R17" s="77" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S17" s="50" t="inlineStr">
+      <c r="S17" s="79" t="inlineStr">
         <is>
           <t xml:space="preserve">2 pages </t>
         </is>
       </c>
-      <c r="T17" s="47" t="inlineStr">
+      <c r="T17" s="76" t="inlineStr">
         <is>
           <t>Box 8, Folder 6, Item 4</t>
         </is>
       </c>
-      <c r="U17" s="47" t="inlineStr">
+      <c r="U17" s="76" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down. Remove plastic sleeve and replace carefully </t>
         </is>
       </c>
-      <c r="V17" s="47" t="inlineStr">
+      <c r="V17" s="76" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F06.04</t>
         </is>
       </c>
-      <c r="W17" s="51" t="n">
+      <c r="W17" s="80" t="n">
         <v>45511</v>
       </c>
-      <c r="X17" s="50" t="inlineStr">
+      <c r="X17" s="79" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y17" s="47" t="n"/>
-      <c r="Z17" s="52" t="inlineStr">
+      <c r="Y17" s="76" t="n"/>
+      <c r="Z17" s="81" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA17" s="47" t="inlineStr">
+      <c r="AA17" s="76" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB17" s="47" t="inlineStr">
+      <c r="AB17" s="76" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC17" s="47" t="n"/>
-      <c r="AD17" s="47" t="n"/>
-      <c r="AE17" s="47" t="n"/>
-      <c r="AF17" s="47" t="n"/>
-      <c r="AG17" s="47" t="n"/>
+      <c r="AC17" s="76" t="n"/>
+      <c r="AD17" s="76" t="n"/>
+      <c r="AE17" s="76" t="n"/>
+      <c r="AF17" s="76" t="n"/>
+      <c r="AG17" s="76" t="n"/>
     </row>
     <row r="18" ht="15.75" customHeight="1" s="5">
-      <c r="A18" s="45" t="inlineStr">
+      <c r="A18" s="74" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B18" s="46" t="n">
+      <c r="B18" s="75" t="n">
         <v>13300</v>
       </c>
-      <c r="C18" s="47" t="n"/>
-      <c r="D18" s="47" t="n"/>
-      <c r="E18" s="47" t="n"/>
-      <c r="F18" s="48" t="inlineStr">
+      <c r="C18" s="76" t="n"/>
+      <c r="D18" s="76" t="n"/>
+      <c r="E18" s="76" t="n"/>
+      <c r="F18" s="77" t="inlineStr">
         <is>
           <t>William Stanley biography, early transcript draft with manuscript inserts</t>
         </is>
       </c>
-      <c r="G18" s="47" t="n"/>
-      <c r="H18" s="48" t="inlineStr">
+      <c r="G18" s="76" t="n"/>
+      <c r="H18" s="77" t="inlineStr">
         <is>
           <t>Annotated Typescript Draft of "The Life of William Stanley" by Thomas C. Martin</t>
         </is>
       </c>
-      <c r="I18" s="47" t="inlineStr">
+      <c r="I18" s="76" t="inlineStr">
         <is>
           <t xml:space="preserve">Includes four drafts of Chapter 8. </t>
         </is>
       </c>
-      <c r="J18" s="45" t="inlineStr">
+      <c r="J18" s="74" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="K18" s="45" t="inlineStr">
+      <c r="K18" s="74" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L18" s="47" t="n"/>
-      <c r="M18" s="45" t="inlineStr">
+      <c r="L18" s="76" t="n"/>
+      <c r="M18" s="74" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N18" s="47" t="n"/>
-      <c r="O18" s="47" t="n"/>
-      <c r="P18" s="49" t="inlineStr">
+      <c r="N18" s="76" t="n"/>
+      <c r="O18" s="76" t="n"/>
+      <c r="P18" s="78" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q18" s="47" t="n"/>
-      <c r="R18" s="48" t="inlineStr">
+      <c r="Q18" s="76" t="n"/>
+      <c r="R18" s="77" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S18" s="50" t="inlineStr">
+      <c r="S18" s="79" t="inlineStr">
         <is>
           <t xml:space="preserve">154 pages </t>
         </is>
       </c>
-      <c r="T18" s="47" t="inlineStr">
+      <c r="T18" s="76" t="inlineStr">
         <is>
           <t>Box 8, Folder 6, Item 5</t>
         </is>
       </c>
-      <c r="U18" s="47" t="inlineStr">
+      <c r="U18" s="76" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down. Use caution to maintain orignal order. Some of the chapters are connected with plastic clips, please remove clips and do not replace them. </t>
         </is>
       </c>
-      <c r="V18" s="47" t="inlineStr">
+      <c r="V18" s="76" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F06.05</t>
         </is>
       </c>
-      <c r="W18" s="51" t="n">
+      <c r="W18" s="80" t="n">
         <v>45511</v>
       </c>
-      <c r="X18" s="50" t="inlineStr">
+      <c r="X18" s="79" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y18" s="47" t="n"/>
-      <c r="Z18" s="52" t="inlineStr">
+      <c r="Y18" s="76" t="n"/>
+      <c r="Z18" s="81" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA18" s="53" t="inlineStr">
+      <c r="AA18" s="82" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB18" s="47" t="inlineStr">
+      <c r="AB18" s="76" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC18" s="47" t="n"/>
-      <c r="AD18" s="47" t="n"/>
-      <c r="AE18" s="47" t="n"/>
-      <c r="AF18" s="47" t="n"/>
-      <c r="AG18" s="47" t="n"/>
+      <c r="AC18" s="76" t="n"/>
+      <c r="AD18" s="76" t="n"/>
+      <c r="AE18" s="76" t="n"/>
+      <c r="AF18" s="76" t="n"/>
+      <c r="AG18" s="76" t="n"/>
     </row>
     <row r="19" ht="15.75" customHeight="1" s="5">
-      <c r="A19" s="45" t="inlineStr">
+      <c r="A19" s="74" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B19" s="46" t="n">
+      <c r="B19" s="75" t="n">
         <v>13301</v>
       </c>
-      <c r="C19" s="47" t="n"/>
-      <c r="D19" s="47" t="n"/>
-      <c r="E19" s="47" t="n"/>
-      <c r="F19" s="48" t="inlineStr">
+      <c r="C19" s="76" t="n"/>
+      <c r="D19" s="76" t="n"/>
+      <c r="E19" s="76" t="n"/>
+      <c r="F19" s="77" t="inlineStr">
         <is>
           <t>William Stanley biography, printers typescript</t>
         </is>
       </c>
-      <c r="G19" s="47" t="n"/>
-      <c r="H19" s="48" t="inlineStr">
+      <c r="G19" s="76" t="n"/>
+      <c r="H19" s="77" t="inlineStr">
         <is>
           <t xml:space="preserve">Printer's Typewritten Text of "The Life of William Stanley" by Thomas C. Martin with Handwritten Notes </t>
         </is>
       </c>
-      <c r="I19" s="47" t="n"/>
-      <c r="J19" s="45" t="inlineStr">
+      <c r="I19" s="76" t="n"/>
+      <c r="J19" s="74" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="K19" s="45" t="inlineStr">
+      <c r="K19" s="74" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L19" s="47" t="n"/>
-      <c r="M19" s="45" t="inlineStr">
+      <c r="L19" s="76" t="n"/>
+      <c r="M19" s="74" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N19" s="47" t="n"/>
-      <c r="O19" s="47" t="n"/>
-      <c r="P19" s="49" t="inlineStr">
+      <c r="N19" s="76" t="n"/>
+      <c r="O19" s="76" t="n"/>
+      <c r="P19" s="78" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q19" s="47" t="n"/>
-      <c r="R19" s="48" t="inlineStr">
+      <c r="Q19" s="76" t="n"/>
+      <c r="R19" s="77" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S19" s="50" t="inlineStr">
+      <c r="S19" s="79" t="inlineStr">
         <is>
           <t xml:space="preserve">99 pages </t>
         </is>
       </c>
-      <c r="T19" s="47" t="inlineStr">
+      <c r="T19" s="76" t="inlineStr">
         <is>
           <t>Box 8, Folder 7</t>
         </is>
       </c>
-      <c r="U19" s="47" t="inlineStr">
+      <c r="U19" s="76" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Up, Paper is Extremely Brittle </t>
         </is>
       </c>
-      <c r="V19" s="47" t="inlineStr">
+      <c r="V19" s="76" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F07</t>
         </is>
       </c>
-      <c r="W19" s="54" t="n">
+      <c r="W19" s="83" t="n">
         <v>45511</v>
       </c>
-      <c r="X19" s="50" t="inlineStr">
+      <c r="X19" s="79" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
-      <c r="Y19" s="47" t="n"/>
-      <c r="Z19" s="52" t="inlineStr">
+      <c r="Y19" s="76" t="n"/>
+      <c r="Z19" s="81" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA19" s="47" t="inlineStr">
+      <c r="AA19" s="76" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB19" s="47" t="inlineStr">
+      <c r="AB19" s="76" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC19" s="47" t="n"/>
-      <c r="AD19" s="47" t="n"/>
-      <c r="AE19" s="47" t="n"/>
-      <c r="AF19" s="47" t="n"/>
-      <c r="AG19" s="47" t="n"/>
+      <c r="AC19" s="76" t="n"/>
+      <c r="AD19" s="76" t="n"/>
+      <c r="AE19" s="76" t="n"/>
+      <c r="AF19" s="76" t="n"/>
+      <c r="AG19" s="76" t="n"/>
     </row>
     <row r="20" ht="15.75" customHeight="1" s="5">
-      <c r="A20" s="45" t="inlineStr">
+      <c r="A20" s="74" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B20" s="46" t="n">
+      <c r="B20" s="75" t="n">
         <v>13339</v>
       </c>
-      <c r="C20" s="47" t="n"/>
-      <c r="D20" s="47" t="n"/>
-      <c r="E20" s="47" t="n"/>
-      <c r="F20" s="48" t="inlineStr">
+      <c r="C20" s="76" t="n"/>
+      <c r="D20" s="76" t="n"/>
+      <c r="E20" s="76" t="n"/>
+      <c r="F20" s="77" t="inlineStr">
         <is>
           <t>"Associations with William Stanley," typescripts</t>
         </is>
       </c>
-      <c r="G20" s="47" t="n"/>
-      <c r="H20" s="48" t="inlineStr">
+      <c r="G20" s="76" t="n"/>
+      <c r="H20" s="77" t="inlineStr">
         <is>
           <t xml:space="preserve">Typescript Draft of "Associates with William Stanley" by Cummings C. Chesney, Including "Play Ball" </t>
         </is>
       </c>
-      <c r="I20" s="47" t="n"/>
-      <c r="J20" s="45" t="inlineStr">
+      <c r="I20" s="76" t="n"/>
+      <c r="J20" s="74" t="inlineStr">
         <is>
           <t>Chesney, Cummings C.</t>
         </is>
       </c>
-      <c r="K20" s="45" t="inlineStr">
+      <c r="K20" s="74" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L20" s="47" t="n"/>
-      <c r="M20" s="45" t="inlineStr">
+      <c r="L20" s="76" t="n"/>
+      <c r="M20" s="74" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N20" s="47" t="n"/>
-      <c r="O20" s="47" t="n"/>
-      <c r="P20" s="49" t="inlineStr">
+      <c r="N20" s="76" t="n"/>
+      <c r="O20" s="76" t="n"/>
+      <c r="P20" s="78" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q20" s="47" t="n"/>
-      <c r="R20" s="48" t="inlineStr">
+      <c r="Q20" s="76" t="n"/>
+      <c r="R20" s="77" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S20" s="50" t="inlineStr">
+      <c r="S20" s="79" t="inlineStr">
         <is>
           <t xml:space="preserve">17 pages </t>
         </is>
       </c>
-      <c r="T20" s="47" t="inlineStr">
+      <c r="T20" s="76" t="inlineStr">
         <is>
           <t xml:space="preserve">Box 8, Folder 8, Item 1 </t>
         </is>
       </c>
-      <c r="U20" s="47" t="inlineStr">
+      <c r="U20" s="76" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down. </t>
         </is>
       </c>
-      <c r="V20" s="47" t="inlineStr">
+      <c r="V20" s="76" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F08.01</t>
         </is>
       </c>
-      <c r="W20" s="54" t="n">
+      <c r="W20" s="83" t="n">
         <v>45511</v>
       </c>
-      <c r="X20" s="47" t="inlineStr">
+      <c r="X20" s="76" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
-      <c r="Y20" s="47" t="n"/>
-      <c r="Z20" s="52" t="inlineStr">
+      <c r="Y20" s="76" t="n"/>
+      <c r="Z20" s="81" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA20" s="47" t="inlineStr">
+      <c r="AA20" s="76" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB20" s="47" t="inlineStr">
+      <c r="AB20" s="76" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC20" s="47" t="n"/>
-      <c r="AD20" s="47" t="n"/>
-      <c r="AE20" s="47" t="n"/>
-      <c r="AF20" s="47" t="n"/>
-      <c r="AG20" s="47" t="n"/>
+      <c r="AC20" s="76" t="n"/>
+      <c r="AD20" s="76" t="n"/>
+      <c r="AE20" s="76" t="n"/>
+      <c r="AF20" s="76" t="n"/>
+      <c r="AG20" s="76" t="n"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="5">
-      <c r="A21" s="45" t="inlineStr">
+      <c r="A21" s="74" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B21" s="46" t="n">
+      <c r="B21" s="75" t="n">
         <v>13339</v>
       </c>
-      <c r="C21" s="47" t="n"/>
-      <c r="D21" s="47" t="n"/>
-      <c r="E21" s="47" t="n"/>
-      <c r="F21" s="48" t="inlineStr">
+      <c r="C21" s="76" t="n"/>
+      <c r="D21" s="76" t="n"/>
+      <c r="E21" s="76" t="n"/>
+      <c r="F21" s="77" t="inlineStr">
         <is>
           <t>"Associations with William Stanley," typescripts</t>
         </is>
       </c>
-      <c r="G21" s="47" t="n"/>
-      <c r="H21" s="48" t="inlineStr">
+      <c r="G21" s="76" t="n"/>
+      <c r="H21" s="77" t="inlineStr">
         <is>
           <t xml:space="preserve">Typescript Draft of "Associates with William Stanley" by Cummings C. Chesney, Untitled </t>
         </is>
       </c>
-      <c r="I21" s="47" t="n"/>
-      <c r="J21" s="45" t="inlineStr">
+      <c r="I21" s="76" t="n"/>
+      <c r="J21" s="74" t="inlineStr">
         <is>
           <t>Chesney, Cummings C.</t>
         </is>
       </c>
-      <c r="K21" s="45" t="inlineStr">
+      <c r="K21" s="74" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L21" s="47" t="n"/>
-      <c r="M21" s="45" t="inlineStr">
+      <c r="L21" s="76" t="n"/>
+      <c r="M21" s="74" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N21" s="47" t="n"/>
-      <c r="O21" s="47" t="n"/>
-      <c r="P21" s="49" t="inlineStr">
+      <c r="N21" s="76" t="n"/>
+      <c r="O21" s="76" t="n"/>
+      <c r="P21" s="78" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q21" s="47" t="n"/>
-      <c r="R21" s="48" t="inlineStr">
+      <c r="Q21" s="76" t="n"/>
+      <c r="R21" s="77" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S21" s="50" t="inlineStr">
+      <c r="S21" s="79" t="inlineStr">
         <is>
           <t xml:space="preserve">13 pages </t>
         </is>
       </c>
-      <c r="T21" s="47" t="inlineStr">
+      <c r="T21" s="76" t="inlineStr">
         <is>
           <t>Box 8, Folder 8, Item 2</t>
         </is>
       </c>
-      <c r="U21" s="47" t="inlineStr">
+      <c r="U21" s="76" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down. </t>
         </is>
       </c>
-      <c r="V21" s="47" t="inlineStr">
+      <c r="V21" s="76" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F08.02</t>
         </is>
       </c>
-      <c r="W21" s="51" t="n">
+      <c r="W21" s="80" t="n">
         <v>45511</v>
       </c>
-      <c r="X21" s="47" t="inlineStr">
+      <c r="X21" s="76" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
-      <c r="Y21" s="47" t="n"/>
-      <c r="Z21" s="52" t="inlineStr">
+      <c r="Y21" s="76" t="n"/>
+      <c r="Z21" s="81" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA21" s="47" t="inlineStr">
+      <c r="AA21" s="76" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB21" s="47" t="inlineStr">
+      <c r="AB21" s="76" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC21" s="47" t="n"/>
-      <c r="AD21" s="47" t="n"/>
-      <c r="AE21" s="47" t="n"/>
-      <c r="AF21" s="47" t="n"/>
-      <c r="AG21" s="47" t="n"/>
+      <c r="AC21" s="76" t="n"/>
+      <c r="AD21" s="76" t="n"/>
+      <c r="AE21" s="76" t="n"/>
+      <c r="AF21" s="76" t="n"/>
+      <c r="AG21" s="76" t="n"/>
     </row>
     <row r="22" ht="15.75" customHeight="1" s="5">
-      <c r="A22" s="45" t="inlineStr">
+      <c r="A22" s="74" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B22" s="46" t="n">
+      <c r="B22" s="75" t="n">
         <v>13339</v>
       </c>
-      <c r="C22" s="47" t="n"/>
-      <c r="D22" s="47" t="n"/>
-      <c r="E22" s="47" t="n"/>
-      <c r="F22" s="48" t="inlineStr">
+      <c r="C22" s="76" t="n"/>
+      <c r="D22" s="76" t="n"/>
+      <c r="E22" s="76" t="n"/>
+      <c r="F22" s="77" t="inlineStr">
         <is>
           <t>"Associations with William Stanley," typescripts</t>
         </is>
       </c>
-      <c r="G22" s="47" t="n"/>
-      <c r="H22" s="48" t="inlineStr">
+      <c r="G22" s="76" t="n"/>
+      <c r="H22" s="77" t="inlineStr">
         <is>
           <t xml:space="preserve">Typescript Draft of "Associates with William Stanley" by Cummings C. Chesney, Untitled from Scientific and Industrial Information Bureau </t>
         </is>
       </c>
-      <c r="I22" s="47" t="n"/>
-      <c r="J22" s="45" t="inlineStr">
+      <c r="I22" s="76" t="n"/>
+      <c r="J22" s="74" t="inlineStr">
         <is>
           <t>Chesney, Cummings C.</t>
         </is>
       </c>
-      <c r="K22" s="45" t="inlineStr">
+      <c r="K22" s="74" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L22" s="47" t="n"/>
-      <c r="M22" s="45" t="inlineStr">
+      <c r="L22" s="76" t="n"/>
+      <c r="M22" s="74" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N22" s="47" t="n"/>
-      <c r="O22" s="47" t="n"/>
-      <c r="P22" s="49" t="inlineStr">
+      <c r="N22" s="76" t="n"/>
+      <c r="O22" s="76" t="n"/>
+      <c r="P22" s="78" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q22" s="47" t="n"/>
-      <c r="R22" s="48" t="inlineStr">
+      <c r="Q22" s="76" t="n"/>
+      <c r="R22" s="77" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S22" s="50" t="inlineStr">
+      <c r="S22" s="79" t="inlineStr">
         <is>
           <t xml:space="preserve">30 pages </t>
         </is>
       </c>
-      <c r="T22" s="47" t="inlineStr">
+      <c r="T22" s="76" t="inlineStr">
         <is>
           <t>Box 8, Folder 8, Item 3</t>
         </is>
       </c>
-      <c r="U22" s="47" t="inlineStr">
+      <c r="U22" s="76" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down. </t>
         </is>
       </c>
-      <c r="V22" s="47" t="inlineStr">
+      <c r="V22" s="76" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F08.03</t>
         </is>
       </c>
-      <c r="W22" s="51" t="n">
+      <c r="W22" s="80" t="n">
         <v>45511</v>
       </c>
-      <c r="X22" s="47" t="inlineStr">
+      <c r="X22" s="76" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
-      <c r="Y22" s="47" t="n"/>
-      <c r="Z22" s="52" t="inlineStr">
+      <c r="Y22" s="76" t="n"/>
+      <c r="Z22" s="81" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA22" s="47" t="inlineStr">
+      <c r="AA22" s="76" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB22" s="47" t="inlineStr">
+      <c r="AB22" s="76" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC22" s="47" t="n"/>
-      <c r="AD22" s="47" t="n"/>
-      <c r="AE22" s="47" t="n"/>
-      <c r="AF22" s="47" t="n"/>
-      <c r="AG22" s="47" t="n"/>
+      <c r="AC22" s="76" t="n"/>
+      <c r="AD22" s="76" t="n"/>
+      <c r="AE22" s="76" t="n"/>
+      <c r="AF22" s="76" t="n"/>
+      <c r="AG22" s="76" t="n"/>
     </row>
     <row r="23" ht="12.75" customHeight="1" s="5">
       <c r="P23" s="38" t="n"/>
@@ -7725,105 +7798,91 @@
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1" s="5">
-      <c r="A13" s="28" t="inlineStr">
+      <c r="A13" s="6" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B13" s="29" t="n">
+      <c r="B13" s="7" t="n">
         <v>13341</v>
       </c>
-      <c r="C13" s="28" t="n"/>
-      <c r="D13" s="28" t="n"/>
-      <c r="E13" s="28" t="n"/>
-      <c r="F13" s="28" t="inlineStr">
+      <c r="C13" s="6" t="n"/>
+      <c r="D13" s="6" t="n"/>
+      <c r="E13" s="6" t="n"/>
+      <c r="F13" s="6" t="inlineStr">
         <is>
           <t>Correspondence regarding National Cyclopedia of American Biography entry on William Stanley</t>
         </is>
       </c>
-      <c r="G13" s="30" t="n"/>
-      <c r="H13" s="31" t="inlineStr">
+      <c r="H13" s="9" t="inlineStr">
         <is>
           <t>Envelope addressed to Dr. Samuel A. Eliot, Editor-in-chief, Biographical History of Massachusetts</t>
         </is>
       </c>
-      <c r="I13" s="30" t="n"/>
-      <c r="J13" s="31" t="inlineStr">
+      <c r="J13" s="9" t="inlineStr">
         <is>
           <t>unknown</t>
         </is>
       </c>
-      <c r="K13" s="30" t="n"/>
-      <c r="L13" s="30" t="n"/>
-      <c r="M13" s="30" t="n"/>
-      <c r="N13" s="28" t="inlineStr">
+      <c r="N13" s="6" t="inlineStr">
         <is>
           <t>Stanley, William, 1858-1916</t>
         </is>
       </c>
-      <c r="O13" s="30" t="n"/>
-      <c r="P13" s="31" t="inlineStr">
+      <c r="P13" s="9" t="inlineStr">
         <is>
           <t>1909-1940</t>
         </is>
       </c>
-      <c r="Q13" s="43" t="n"/>
-      <c r="R13" s="30" t="n"/>
-      <c r="S13" s="31" t="inlineStr">
+      <c r="Q13" s="38" t="n"/>
+      <c r="S13" s="9" t="inlineStr">
         <is>
           <t>No Copyright - United States</t>
         </is>
       </c>
-      <c r="T13" s="31" t="inlineStr">
+      <c r="T13" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">5 pages </t>
         </is>
       </c>
-      <c r="U13" s="28" t="inlineStr">
+      <c r="U13" s="6" t="inlineStr">
         <is>
           <t>Box 9, Folder 2, Item 6</t>
         </is>
       </c>
-      <c r="V13" s="33" t="inlineStr">
+      <c r="V13" s="8" t="inlineStr">
         <is>
           <t>Glass down</t>
         </is>
       </c>
-      <c r="W13" s="31" t="inlineStr">
+      <c r="W13" s="9" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B09.F02.06</t>
         </is>
       </c>
-      <c r="X13" s="34" t="n">
+      <c r="X13" s="16" t="n">
         <v>45513</v>
       </c>
-      <c r="Y13" s="31" t="inlineStr">
+      <c r="Y13" s="9" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Z13" s="30" t="n"/>
-      <c r="AA13" s="28" t="inlineStr">
+      <c r="AA13" s="6" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AB13" s="30" t="inlineStr">
+      <c r="AB13" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AC13" s="30" t="inlineStr">
+      <c r="AC13" t="inlineStr">
         <is>
           <t>Incorrect page count</t>
         </is>
       </c>
-      <c r="AD13" s="30" t="n"/>
-      <c r="AE13" s="30" t="n"/>
-      <c r="AF13" s="30" t="n"/>
-      <c r="AG13" s="30" t="n"/>
-      <c r="AH13" s="30" t="n"/>
-      <c r="AI13" s="30" t="n"/>
     </row>
     <row r="14" ht="15.75" customHeight="1" s="5">
       <c r="A14" s="6" t="inlineStr">
@@ -9148,101 +9207,84 @@
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1" s="5">
-      <c r="A30" s="28" t="inlineStr">
+      <c r="A30" s="6" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B30" s="29" t="n">
+      <c r="B30" s="7" t="n">
         <v>13341</v>
       </c>
-      <c r="C30" s="30" t="n"/>
-      <c r="D30" s="30" t="n"/>
-      <c r="E30" s="30" t="n"/>
-      <c r="F30" s="28" t="inlineStr">
+      <c r="F30" s="6" t="inlineStr">
         <is>
           <t>Correspondence regarding National Cyclopedia of American Biography entry on William Stanley</t>
         </is>
       </c>
-      <c r="G30" s="30" t="n"/>
-      <c r="H30" s="31" t="inlineStr">
+      <c r="H30" s="9" t="inlineStr">
         <is>
           <t>American Inventors pamphlet</t>
         </is>
       </c>
-      <c r="I30" s="30" t="n"/>
-      <c r="J30" s="31" t="inlineStr">
+      <c r="J30" s="9" t="inlineStr">
         <is>
           <t>The National Cyclopedia of American Biography</t>
         </is>
       </c>
-      <c r="K30" s="30" t="n"/>
-      <c r="L30" s="30" t="n"/>
-      <c r="M30" s="30" t="n"/>
-      <c r="N30" s="28" t="inlineStr">
+      <c r="N30" s="6" t="inlineStr">
         <is>
           <t>Stanley, William, 1858-1916</t>
         </is>
       </c>
-      <c r="O30" s="30" t="n"/>
-      <c r="P30" s="31" t="inlineStr">
+      <c r="P30" s="9" t="inlineStr">
         <is>
           <t>1910-1920</t>
         </is>
       </c>
-      <c r="Q30" s="43" t="n"/>
-      <c r="R30" s="30" t="n"/>
-      <c r="S30" s="31" t="inlineStr">
+      <c r="Q30" s="38" t="n"/>
+      <c r="S30" s="9" t="inlineStr">
         <is>
           <t>Copyright Undetermined</t>
         </is>
       </c>
-      <c r="T30" s="31" t="n"/>
-      <c r="U30" s="28" t="inlineStr">
+      <c r="T30" s="9" t="n"/>
+      <c r="U30" s="6" t="inlineStr">
         <is>
           <t>Box 9, Folder 2, Item 23</t>
         </is>
       </c>
-      <c r="V30" s="33" t="inlineStr">
+      <c r="V30" s="8" t="inlineStr">
         <is>
           <t>Glass down</t>
         </is>
       </c>
-      <c r="W30" s="31" t="inlineStr">
+      <c r="W30" s="9" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B09.F02.23</t>
         </is>
       </c>
-      <c r="X30" s="34" t="n">
+      <c r="X30" s="16" t="n">
         <v>45513</v>
       </c>
-      <c r="Y30" s="31" t="inlineStr">
+      <c r="Y30" s="9" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Z30" s="30" t="n"/>
-      <c r="AA30" s="28" t="inlineStr">
+      <c r="AA30" s="6" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AB30" s="30" t="inlineStr">
+      <c r="AB30" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AC30" s="30" t="inlineStr">
+      <c r="AC30" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AD30" s="30" t="n"/>
-      <c r="AE30" s="30" t="n"/>
-      <c r="AF30" s="30" t="n"/>
-      <c r="AG30" s="30" t="n"/>
-      <c r="AH30" s="30" t="n"/>
-      <c r="AI30" s="30" t="n"/>
     </row>
     <row r="31" ht="15.75" customHeight="1" s="5">
       <c r="A31" s="6" t="inlineStr">
@@ -16796,105 +16838,88 @@
       </c>
     </row>
     <row r="122" ht="15" customHeight="1" s="5">
-      <c r="A122" s="28" t="inlineStr">
+      <c r="A122" s="6" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B122" s="29" t="n">
+      <c r="B122" s="7" t="n">
         <v>13344</v>
       </c>
-      <c r="C122" s="30" t="n"/>
-      <c r="D122" s="30" t="n"/>
-      <c r="E122" s="30" t="n"/>
-      <c r="F122" s="28" t="inlineStr">
+      <c r="F122" s="6" t="inlineStr">
         <is>
           <t>Correspondence regarding William Stanley biography</t>
         </is>
       </c>
-      <c r="G122" s="30" t="n"/>
-      <c r="H122" s="31" t="inlineStr">
+      <c r="H122" s="9" t="inlineStr">
         <is>
           <t>Table of contents draft for Life of William Stanley manuscript</t>
         </is>
       </c>
-      <c r="I122" s="30" t="n"/>
-      <c r="J122" s="31" t="inlineStr">
+      <c r="J122" s="9" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="K122" s="30" t="n"/>
-      <c r="L122" s="30" t="n"/>
-      <c r="M122" s="30" t="n"/>
-      <c r="N122" s="31" t="inlineStr">
+      <c r="N122" s="9" t="inlineStr">
         <is>
           <t>Stanley, William, 1858-1916</t>
         </is>
       </c>
-      <c r="O122" s="30" t="n"/>
-      <c r="P122" s="31" t="inlineStr">
+      <c r="P122" s="9" t="inlineStr">
         <is>
           <t>1922-1924</t>
         </is>
       </c>
-      <c r="Q122" s="43" t="n"/>
-      <c r="R122" s="30" t="n"/>
-      <c r="S122" s="31" t="inlineStr">
+      <c r="Q122" s="38" t="n"/>
+      <c r="S122" s="9" t="inlineStr">
         <is>
           <t>No Copyright - United States</t>
         </is>
       </c>
-      <c r="T122" s="31" t="inlineStr">
+      <c r="T122" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">1 page </t>
         </is>
       </c>
-      <c r="U122" s="28" t="inlineStr">
+      <c r="U122" s="6" t="inlineStr">
         <is>
           <t>Box 9, Folder 5, Item 67</t>
         </is>
       </c>
-      <c r="V122" s="33" t="inlineStr">
+      <c r="V122" s="8" t="inlineStr">
         <is>
           <t>Glass down</t>
         </is>
       </c>
-      <c r="W122" s="31" t="inlineStr">
+      <c r="W122" s="9" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B09.F05.67</t>
         </is>
       </c>
-      <c r="X122" s="34" t="n">
+      <c r="X122" s="16" t="n">
         <v>45523</v>
       </c>
-      <c r="Y122" s="31" t="inlineStr">
+      <c r="Y122" s="9" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Z122" s="30" t="n"/>
-      <c r="AA122" s="28" t="inlineStr">
+      <c r="AA122" s="6" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AB122" s="30" t="inlineStr">
+      <c r="AB122" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AC122" s="30" t="inlineStr">
+      <c r="AC122" t="inlineStr">
         <is>
           <t>Incorrect page count</t>
         </is>
       </c>
-      <c r="AD122" s="30" t="n"/>
-      <c r="AE122" s="30" t="n"/>
-      <c r="AF122" s="30" t="n"/>
-      <c r="AG122" s="30" t="n"/>
-      <c r="AH122" s="30" t="n"/>
-      <c r="AI122" s="30" t="n"/>
     </row>
     <row r="123" ht="15" customHeight="1" s="5">
       <c r="A123" s="6" t="inlineStr">
@@ -17952,105 +17977,105 @@
       </c>
     </row>
     <row r="136" ht="15" customHeight="1" s="5">
-      <c r="A136" s="52" t="inlineStr">
+      <c r="A136" s="81" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B136" s="55" t="n">
+      <c r="B136" s="84" t="n">
         <v>13344</v>
       </c>
-      <c r="C136" s="52" t="n"/>
-      <c r="D136" s="52" t="n"/>
-      <c r="E136" s="52" t="n"/>
-      <c r="F136" s="52" t="inlineStr">
+      <c r="C136" s="81" t="n"/>
+      <c r="D136" s="81" t="n"/>
+      <c r="E136" s="81" t="n"/>
+      <c r="F136" s="81" t="inlineStr">
         <is>
           <t>Correspondence regarding William Stanley biography</t>
         </is>
       </c>
-      <c r="G136" s="56" t="n"/>
-      <c r="H136" s="50" t="inlineStr">
+      <c r="G136" s="85" t="n"/>
+      <c r="H136" s="79" t="inlineStr">
         <is>
           <t>Letter from C. C. Chesney to T. C. Martin, November 13, 1922, with enclosures</t>
         </is>
       </c>
-      <c r="I136" s="50" t="inlineStr">
+      <c r="I136" s="79" t="inlineStr">
         <is>
           <t>Enclosures: Letter from F. Darlington to T. C. Martin, November 5, 1922 and letter from  Philip G. Gossler to T. C. Martin, November 6, 1922</t>
         </is>
       </c>
-      <c r="J136" s="50" t="inlineStr">
+      <c r="J136" s="79" t="inlineStr">
         <is>
           <t>Chesney, Cummings C.;Darlington, Frederick;Gossler, Philip G.</t>
         </is>
       </c>
-      <c r="K136" s="56" t="n"/>
-      <c r="L136" s="56" t="n"/>
-      <c r="M136" s="56" t="n"/>
-      <c r="N136" s="50" t="inlineStr">
+      <c r="K136" s="85" t="n"/>
+      <c r="L136" s="85" t="n"/>
+      <c r="M136" s="85" t="n"/>
+      <c r="N136" s="79" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924;Stanley, William, 1858-1916</t>
         </is>
       </c>
-      <c r="O136" s="56" t="n"/>
-      <c r="P136" s="56" t="n"/>
-      <c r="Q136" s="57" t="inlineStr">
+      <c r="O136" s="85" t="n"/>
+      <c r="P136" s="85" t="n"/>
+      <c r="Q136" s="86" t="inlineStr">
         <is>
           <t>1922-11-06;1922-11-08;1922-11-13</t>
         </is>
       </c>
-      <c r="R136" s="56" t="n"/>
-      <c r="S136" s="50" t="inlineStr">
+      <c r="R136" s="85" t="n"/>
+      <c r="S136" s="79" t="inlineStr">
         <is>
           <t>No Copyright - United States</t>
         </is>
       </c>
-      <c r="T136" s="56" t="n"/>
-      <c r="U136" s="52" t="inlineStr">
+      <c r="T136" s="85" t="n"/>
+      <c r="U136" s="81" t="inlineStr">
         <is>
           <t>Box 9, Folder 5, Item 81</t>
         </is>
       </c>
-      <c r="V136" s="58" t="inlineStr">
+      <c r="V136" s="87" t="inlineStr">
         <is>
           <t>Glass down</t>
         </is>
       </c>
-      <c r="W136" s="50" t="inlineStr">
+      <c r="W136" s="79" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B09.F05.81</t>
         </is>
       </c>
-      <c r="X136" s="59" t="n">
+      <c r="X136" s="88" t="n">
         <v>45523</v>
       </c>
-      <c r="Y136" s="50" t="inlineStr">
+      <c r="Y136" s="79" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Z136" s="56" t="n"/>
-      <c r="AA136" s="52" t="inlineStr">
+      <c r="Z136" s="85" t="n"/>
+      <c r="AA136" s="81" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AB136" s="56" t="inlineStr">
+      <c r="AB136" s="85" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AC136" s="56" t="inlineStr">
+      <c r="AC136" s="85" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AD136" s="56" t="n"/>
-      <c r="AE136" s="56" t="n"/>
-      <c r="AF136" s="56" t="n"/>
-      <c r="AG136" s="56" t="n"/>
-      <c r="AH136" s="56" t="n"/>
-      <c r="AI136" s="56" t="n"/>
+      <c r="AD136" s="85" t="n"/>
+      <c r="AE136" s="85" t="n"/>
+      <c r="AF136" s="85" t="n"/>
+      <c r="AG136" s="85" t="n"/>
+      <c r="AH136" s="85" t="n"/>
+      <c r="AI136" s="85" t="n"/>
     </row>
     <row r="137" ht="15" customHeight="1" s="5">
       <c r="A137" s="6" t="inlineStr">
@@ -18290,99 +18315,83 @@
       </c>
     </row>
     <row r="140" ht="15" customHeight="1" s="5">
-      <c r="A140" s="28" t="inlineStr">
+      <c r="A140" s="6" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B140" s="29" t="n">
+      <c r="B140" s="7" t="n">
         <v>13344</v>
       </c>
-      <c r="C140" s="28" t="n"/>
-      <c r="D140" s="28" t="n"/>
-      <c r="E140" s="28" t="n"/>
-      <c r="F140" s="28" t="inlineStr">
+      <c r="C140" s="6" t="n"/>
+      <c r="D140" s="6" t="n"/>
+      <c r="E140" s="6" t="n"/>
+      <c r="F140" s="6" t="inlineStr">
         <is>
           <t>Correspondence regarding William Stanley biography</t>
         </is>
       </c>
-      <c r="G140" s="30" t="n"/>
-      <c r="H140" s="31" t="inlineStr">
+      <c r="H140" s="9" t="inlineStr">
         <is>
           <t>Letter from [T. C. Martin] to C. C. Chesney, October 11, 1922</t>
         </is>
       </c>
-      <c r="I140" s="30" t="n"/>
-      <c r="J140" s="31" t="inlineStr">
+      <c r="J140" s="9" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="K140" s="30" t="n"/>
-      <c r="L140" s="30" t="n"/>
-      <c r="M140" s="30" t="n"/>
-      <c r="N140" s="31" t="inlineStr">
+      <c r="N140" s="9" t="inlineStr">
         <is>
           <t>Chesney, Cummings C.;Stanley, William, 1858-1916</t>
         </is>
       </c>
-      <c r="O140" s="30" t="n"/>
-      <c r="P140" s="30" t="n"/>
-      <c r="Q140" s="44" t="n">
+      <c r="Q140" s="40" t="n">
         <v>8320</v>
       </c>
-      <c r="R140" s="30" t="n"/>
-      <c r="S140" s="31" t="inlineStr">
+      <c r="S140" s="9" t="inlineStr">
         <is>
           <t>No Copyright - United States</t>
         </is>
       </c>
-      <c r="T140" s="30" t="n"/>
-      <c r="U140" s="28" t="inlineStr">
+      <c r="U140" s="6" t="inlineStr">
         <is>
           <t>Box 9, Folder 5, Item 85</t>
         </is>
       </c>
-      <c r="V140" s="33" t="inlineStr">
+      <c r="V140" s="8" t="inlineStr">
         <is>
           <t>Glass down</t>
         </is>
       </c>
-      <c r="W140" s="31" t="inlineStr">
+      <c r="W140" s="9" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B09.F05.85</t>
         </is>
       </c>
-      <c r="X140" s="34" t="n">
+      <c r="X140" s="16" t="n">
         <v>45523</v>
       </c>
-      <c r="Y140" s="31" t="inlineStr">
+      <c r="Y140" s="9" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Z140" s="30" t="n"/>
-      <c r="AA140" s="28" t="inlineStr">
+      <c r="AA140" s="6" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AB140" s="30" t="inlineStr">
+      <c r="AB140" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AC140" s="30" t="inlineStr">
+      <c r="AC140" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AD140" s="30" t="n"/>
-      <c r="AE140" s="30" t="n"/>
-      <c r="AF140" s="30" t="n"/>
-      <c r="AG140" s="30" t="n"/>
-      <c r="AH140" s="30" t="n"/>
-      <c r="AI140" s="30" t="n"/>
     </row>
     <row r="141" ht="15" customHeight="1" s="5">
       <c r="A141" s="6" t="inlineStr">
@@ -22908,101 +22917,101 @@
       </c>
     </row>
     <row r="198" ht="15" customHeight="1" s="5">
-      <c r="A198" s="52" t="inlineStr">
+      <c r="A198" s="81" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B198" s="55" t="n">
+      <c r="B198" s="84" t="n">
         <v>13346</v>
       </c>
-      <c r="C198" s="52" t="n"/>
-      <c r="D198" s="52" t="n"/>
-      <c r="E198" s="52" t="n"/>
-      <c r="F198" s="52" t="inlineStr">
+      <c r="C198" s="81" t="n"/>
+      <c r="D198" s="81" t="n"/>
+      <c r="E198" s="81" t="n"/>
+      <c r="F198" s="81" t="inlineStr">
         <is>
           <t>Biographical articles and brochures</t>
         </is>
       </c>
-      <c r="G198" s="56" t="n"/>
-      <c r="H198" s="52" t="inlineStr">
+      <c r="G198" s="85" t="n"/>
+      <c r="H198" s="81" t="inlineStr">
         <is>
           <t>Biographical articles and brochures, Item 9</t>
         </is>
       </c>
-      <c r="I198" s="56" t="n"/>
-      <c r="J198" s="50" t="inlineStr">
+      <c r="I198" s="85" t="n"/>
+      <c r="J198" s="79" t="inlineStr">
         <is>
           <t>unknown</t>
         </is>
       </c>
-      <c r="K198" s="56" t="n"/>
-      <c r="L198" s="56" t="n"/>
-      <c r="M198" s="56" t="n"/>
-      <c r="N198" s="50" t="inlineStr">
+      <c r="K198" s="85" t="n"/>
+      <c r="L198" s="85" t="n"/>
+      <c r="M198" s="85" t="n"/>
+      <c r="N198" s="79" t="inlineStr">
         <is>
           <t>Stanley, William, 1858-1916</t>
         </is>
       </c>
-      <c r="O198" s="56" t="n"/>
-      <c r="P198" s="56" t="n"/>
-      <c r="Q198" s="57" t="inlineStr">
+      <c r="O198" s="85" t="n"/>
+      <c r="P198" s="85" t="n"/>
+      <c r="Q198" s="86" t="inlineStr">
         <is>
           <t>unknown</t>
         </is>
       </c>
-      <c r="R198" s="56" t="n"/>
-      <c r="S198" s="50" t="inlineStr">
+      <c r="R198" s="85" t="n"/>
+      <c r="S198" s="79" t="inlineStr">
         <is>
           <t>Copyright Undetermined</t>
         </is>
       </c>
-      <c r="T198" s="56" t="n"/>
-      <c r="U198" s="50" t="inlineStr">
+      <c r="T198" s="85" t="n"/>
+      <c r="U198" s="79" t="inlineStr">
         <is>
           <t>Box 9, Folder 8, Item 9</t>
         </is>
       </c>
-      <c r="V198" s="58" t="inlineStr">
+      <c r="V198" s="87" t="inlineStr">
         <is>
           <t>Glass down</t>
         </is>
       </c>
-      <c r="W198" s="50" t="inlineStr">
+      <c r="W198" s="79" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B09.F08.09</t>
         </is>
       </c>
-      <c r="X198" s="59" t="n">
+      <c r="X198" s="88" t="n">
         <v>45524</v>
       </c>
-      <c r="Y198" s="50" t="inlineStr">
+      <c r="Y198" s="79" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Z198" s="56" t="n"/>
-      <c r="AA198" s="52" t="inlineStr">
+      <c r="Z198" s="85" t="n"/>
+      <c r="AA198" s="81" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AB198" s="56" t="inlineStr">
+      <c r="AB198" s="85" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AC198" s="56" t="inlineStr">
+      <c r="AC198" s="85" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AD198" s="56" t="n"/>
-      <c r="AE198" s="56" t="n"/>
-      <c r="AF198" s="56" t="n"/>
-      <c r="AG198" s="56" t="n"/>
-      <c r="AH198" s="56" t="n"/>
-      <c r="AI198" s="56" t="n"/>
+      <c r="AD198" s="85" t="n"/>
+      <c r="AE198" s="85" t="n"/>
+      <c r="AF198" s="85" t="n"/>
+      <c r="AG198" s="85" t="n"/>
+      <c r="AH198" s="85" t="n"/>
+      <c r="AI198" s="85" t="n"/>
     </row>
     <row r="199" ht="15" customHeight="1" s="5">
       <c r="A199" s="6" t="inlineStr">

</xml_diff>

<commit_message>
changed the name of the UI file
</commit_message>
<xml_diff>
--- a/app/spreadsheets/sample.xlsx
+++ b/app/spreadsheets/sample.xlsx
@@ -57,7 +57,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill/>
     </fill>
@@ -100,6 +100,18 @@
         <bgColor rgb="FFE79DFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA365FF"/>
+        <bgColor rgb="FFA365FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3CB1"/>
+        <bgColor rgb="FFFF3CB1"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -113,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -310,6 +322,52 @@
     </xf>
     <xf numFmtId="165" fontId="2" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="2" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="3" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,95 +827,95 @@
       <c r="AG1" s="4" t="n"/>
     </row>
     <row r="2" ht="15.75" customHeight="1" s="5">
-      <c r="A2" s="89" t="inlineStr">
+      <c r="A2" s="22" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B2" s="90" t="n">
+      <c r="B2" s="23" t="n">
         <v>13295</v>
       </c>
-      <c r="C2" s="91" t="n"/>
-      <c r="D2" s="91" t="n"/>
-      <c r="E2" s="91" t="n"/>
-      <c r="F2" s="92" t="inlineStr">
+      <c r="C2" s="24" t="n"/>
+      <c r="D2" s="24" t="n"/>
+      <c r="E2" s="24" t="n"/>
+      <c r="F2" s="25" t="inlineStr">
         <is>
           <t>Technical papers and other research articles by William Stanley</t>
         </is>
       </c>
-      <c r="G2" s="91" t="n"/>
-      <c r="H2" s="92" t="inlineStr">
+      <c r="G2" s="24" t="n"/>
+      <c r="H2" s="25" t="inlineStr">
         <is>
           <t xml:space="preserve">Stanley Ferrostat Vaccum Products Pamphlet </t>
         </is>
       </c>
-      <c r="I2" s="91" t="n"/>
-      <c r="J2" s="91" t="n"/>
-      <c r="K2" s="91" t="n"/>
-      <c r="L2" s="91" t="n"/>
-      <c r="M2" s="89" t="inlineStr">
+      <c r="I2" s="24" t="n"/>
+      <c r="J2" s="24" t="n"/>
+      <c r="K2" s="24" t="n"/>
+      <c r="L2" s="24" t="n"/>
+      <c r="M2" s="22" t="inlineStr">
         <is>
           <t>1887 - 1913</t>
         </is>
       </c>
-      <c r="N2" s="91" t="n"/>
-      <c r="O2" s="91" t="n"/>
-      <c r="P2" s="93" t="n">
+      <c r="N2" s="24" t="n"/>
+      <c r="O2" s="24" t="n"/>
+      <c r="P2" s="42" t="n">
         <v>1913</v>
       </c>
-      <c r="Q2" s="91" t="n"/>
-      <c r="R2" s="92" t="inlineStr">
+      <c r="Q2" s="24" t="n"/>
+      <c r="R2" s="25" t="inlineStr">
         <is>
           <t xml:space="preserve">No Copyright - United States </t>
         </is>
       </c>
-      <c r="S2" s="91" t="inlineStr">
+      <c r="S2" s="24" t="inlineStr">
         <is>
           <t xml:space="preserve">2 pages </t>
         </is>
       </c>
-      <c r="T2" s="91" t="inlineStr">
+      <c r="T2" s="24" t="inlineStr">
         <is>
           <t xml:space="preserve">Box 8, Folder 1, Item 1 </t>
         </is>
       </c>
-      <c r="U2" s="91" t="inlineStr">
+      <c r="U2" s="24" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down. </t>
         </is>
       </c>
-      <c r="V2" s="91" t="n">
+      <c r="V2" s="24" t="n">
         <v>0</v>
       </c>
-      <c r="W2" s="94" t="n">
+      <c r="W2" s="27" t="n">
         <v>45506</v>
       </c>
-      <c r="X2" s="91" t="inlineStr">
+      <c r="X2" s="24" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
-      <c r="Y2" s="91" t="n"/>
-      <c r="Z2" s="95" t="inlineStr">
+      <c r="Y2" s="24" t="n"/>
+      <c r="Z2" s="28" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA2" s="91" t="inlineStr">
+      <c r="AA2" s="24" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB2" s="91" t="inlineStr">
+      <c r="AB2" s="24" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC2" s="91" t="n"/>
-      <c r="AD2" s="91" t="n"/>
-      <c r="AE2" s="91" t="n"/>
-      <c r="AF2" s="91" t="n"/>
-      <c r="AG2" s="91" t="n"/>
+      <c r="AC2" s="24" t="n"/>
+      <c r="AD2" s="24" t="n"/>
+      <c r="AE2" s="24" t="n"/>
+      <c r="AF2" s="24" t="n"/>
+      <c r="AG2" s="24" t="n"/>
     </row>
     <row r="3" ht="15.75" customHeight="1" s="5">
       <c r="A3" s="1" t="inlineStr">
@@ -1839,935 +1897,935 @@
       <c r="AG13" s="4" t="n"/>
     </row>
     <row r="14" ht="15.75" customHeight="1" s="5">
-      <c r="A14" s="74" t="inlineStr">
+      <c r="A14" s="103" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B14" s="75" t="n">
+      <c r="B14" s="104" t="n">
         <v>13300</v>
       </c>
-      <c r="C14" s="76" t="n"/>
-      <c r="D14" s="76" t="n"/>
-      <c r="E14" s="76" t="n"/>
-      <c r="F14" s="77" t="inlineStr">
+      <c r="C14" s="105" t="n"/>
+      <c r="D14" s="105" t="n"/>
+      <c r="E14" s="105" t="n"/>
+      <c r="F14" s="106" t="inlineStr">
         <is>
           <t>William Stanley biography, early transcript draft with manuscript inserts</t>
         </is>
       </c>
-      <c r="G14" s="76" t="n"/>
-      <c r="H14" s="77" t="inlineStr">
+      <c r="G14" s="105" t="n"/>
+      <c r="H14" s="106" t="inlineStr">
         <is>
           <t>Sections of Typescript Draft of "The Life of William Stanley" by Thomas C. Martin, "Stanley as Inventor and Manufacturer at Pittsfield"</t>
         </is>
       </c>
-      <c r="I14" s="76" t="n"/>
-      <c r="J14" s="74" t="inlineStr">
+      <c r="I14" s="105" t="n"/>
+      <c r="J14" s="103" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="K14" s="74" t="inlineStr">
+      <c r="K14" s="103" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L14" s="76" t="n"/>
-      <c r="M14" s="74" t="inlineStr">
+      <c r="L14" s="105" t="n"/>
+      <c r="M14" s="103" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N14" s="76" t="n"/>
-      <c r="O14" s="76" t="n"/>
-      <c r="P14" s="78" t="inlineStr">
+      <c r="N14" s="105" t="n"/>
+      <c r="O14" s="105" t="n"/>
+      <c r="P14" s="107" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q14" s="76" t="n"/>
-      <c r="R14" s="77" t="inlineStr">
+      <c r="Q14" s="105" t="n"/>
+      <c r="R14" s="106" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S14" s="79" t="inlineStr">
+      <c r="S14" s="108" t="inlineStr">
         <is>
           <t xml:space="preserve">14 pages </t>
         </is>
       </c>
-      <c r="T14" s="76" t="inlineStr">
+      <c r="T14" s="105" t="inlineStr">
         <is>
           <t xml:space="preserve">Box 8, Folder 6, Item 1  </t>
         </is>
       </c>
-      <c r="U14" s="76" t="inlineStr">
+      <c r="U14" s="105" t="inlineStr">
         <is>
           <t>Glass Down. Goes until Page 14. Please make sure you scan complete section.</t>
         </is>
       </c>
-      <c r="V14" s="76" t="inlineStr">
+      <c r="V14" s="105" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F06.01</t>
         </is>
       </c>
-      <c r="W14" s="80" t="n">
+      <c r="W14" s="109" t="n">
         <v>45510</v>
       </c>
-      <c r="X14" s="79" t="inlineStr">
+      <c r="X14" s="108" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y14" s="76" t="n"/>
-      <c r="Z14" s="81" t="inlineStr">
+      <c r="Y14" s="105" t="n"/>
+      <c r="Z14" s="110" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA14" s="76" t="inlineStr">
+      <c r="AA14" s="105" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB14" s="76" t="inlineStr">
+      <c r="AB14" s="105" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC14" s="76" t="n"/>
-      <c r="AD14" s="76" t="n"/>
-      <c r="AE14" s="76" t="n"/>
-      <c r="AF14" s="76" t="n"/>
-      <c r="AG14" s="76" t="n"/>
+      <c r="AC14" s="105" t="n"/>
+      <c r="AD14" s="105" t="n"/>
+      <c r="AE14" s="105" t="n"/>
+      <c r="AF14" s="105" t="n"/>
+      <c r="AG14" s="105" t="n"/>
     </row>
     <row r="15" ht="15.75" customHeight="1" s="5">
-      <c r="A15" s="74" t="inlineStr">
+      <c r="A15" s="103" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B15" s="75" t="n">
+      <c r="B15" s="104" t="n">
         <v>13300</v>
       </c>
-      <c r="C15" s="76" t="n"/>
-      <c r="D15" s="76" t="n"/>
-      <c r="E15" s="76" t="n"/>
-      <c r="F15" s="77" t="inlineStr">
+      <c r="C15" s="105" t="n"/>
+      <c r="D15" s="105" t="n"/>
+      <c r="E15" s="105" t="n"/>
+      <c r="F15" s="106" t="inlineStr">
         <is>
           <t>William Stanley biography, early transcript draft with manuscript inserts</t>
         </is>
       </c>
-      <c r="G15" s="76" t="n"/>
-      <c r="H15" s="77" t="inlineStr">
+      <c r="G15" s="105" t="n"/>
+      <c r="H15" s="106" t="inlineStr">
         <is>
           <t xml:space="preserve">Sections of Typescript Draft of "The Life of William Stanley" by Thomas C. Martin, Untitiled from Scientific and Industrial Information Bureau </t>
         </is>
       </c>
-      <c r="I15" s="76" t="n"/>
-      <c r="J15" s="74" t="inlineStr">
+      <c r="I15" s="105" t="n"/>
+      <c r="J15" s="103" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="K15" s="74" t="inlineStr">
+      <c r="K15" s="103" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L15" s="76" t="n"/>
-      <c r="M15" s="74" t="inlineStr">
+      <c r="L15" s="105" t="n"/>
+      <c r="M15" s="103" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N15" s="76" t="n"/>
-      <c r="O15" s="76" t="n"/>
-      <c r="P15" s="78" t="inlineStr">
+      <c r="N15" s="105" t="n"/>
+      <c r="O15" s="105" t="n"/>
+      <c r="P15" s="107" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q15" s="76" t="n"/>
-      <c r="R15" s="77" t="inlineStr">
+      <c r="Q15" s="105" t="n"/>
+      <c r="R15" s="106" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S15" s="79" t="inlineStr">
+      <c r="S15" s="108" t="inlineStr">
         <is>
           <t xml:space="preserve">21 pages </t>
         </is>
       </c>
-      <c r="T15" s="76" t="inlineStr">
+      <c r="T15" s="105" t="inlineStr">
         <is>
           <t>Box 8, Folder 6, Item 2</t>
         </is>
       </c>
-      <c r="U15" s="76" t="inlineStr">
+      <c r="U15" s="105" t="inlineStr">
         <is>
           <t>Glass Down. Use white paper as marker for section. Please make sure you scan complete section.</t>
         </is>
       </c>
-      <c r="V15" s="76" t="inlineStr">
+      <c r="V15" s="105" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F06.02</t>
         </is>
       </c>
-      <c r="W15" s="80" t="n">
+      <c r="W15" s="109" t="n">
         <v>45511</v>
       </c>
-      <c r="X15" s="79" t="inlineStr">
+      <c r="X15" s="108" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y15" s="76" t="n"/>
-      <c r="Z15" s="81" t="inlineStr">
+      <c r="Y15" s="105" t="n"/>
+      <c r="Z15" s="110" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA15" s="76" t="inlineStr">
+      <c r="AA15" s="105" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB15" s="76" t="inlineStr">
+      <c r="AB15" s="105" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC15" s="76" t="n"/>
-      <c r="AD15" s="76" t="n"/>
-      <c r="AE15" s="76" t="n"/>
-      <c r="AF15" s="76" t="n"/>
-      <c r="AG15" s="76" t="n"/>
+      <c r="AC15" s="105" t="n"/>
+      <c r="AD15" s="105" t="n"/>
+      <c r="AE15" s="105" t="n"/>
+      <c r="AF15" s="105" t="n"/>
+      <c r="AG15" s="105" t="n"/>
     </row>
     <row r="16" ht="15.75" customHeight="1" s="5">
-      <c r="A16" s="74" t="inlineStr">
+      <c r="A16" s="103" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B16" s="75" t="n">
+      <c r="B16" s="104" t="n">
         <v>13300</v>
       </c>
-      <c r="C16" s="76" t="n"/>
-      <c r="D16" s="76" t="n"/>
-      <c r="E16" s="76" t="n"/>
-      <c r="F16" s="77" t="inlineStr">
+      <c r="C16" s="105" t="n"/>
+      <c r="D16" s="105" t="n"/>
+      <c r="E16" s="105" t="n"/>
+      <c r="F16" s="106" t="inlineStr">
         <is>
           <t>William Stanley biography, early transcript draft with manuscript inserts</t>
         </is>
       </c>
-      <c r="G16" s="76" t="n"/>
-      <c r="H16" s="77" t="inlineStr">
+      <c r="G16" s="105" t="n"/>
+      <c r="H16" s="106" t="inlineStr">
         <is>
           <t xml:space="preserve">Sections of Typescript Draft of "The Life of William Stanley" by Thomas C. Martin, Untitiled </t>
         </is>
       </c>
-      <c r="I16" s="76" t="n"/>
-      <c r="J16" s="74" t="inlineStr">
+      <c r="I16" s="105" t="n"/>
+      <c r="J16" s="103" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="K16" s="74" t="inlineStr">
+      <c r="K16" s="103" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L16" s="76" t="n"/>
-      <c r="M16" s="74" t="inlineStr">
+      <c r="L16" s="105" t="n"/>
+      <c r="M16" s="103" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N16" s="76" t="n"/>
-      <c r="O16" s="76" t="n"/>
-      <c r="P16" s="78" t="inlineStr">
+      <c r="N16" s="105" t="n"/>
+      <c r="O16" s="105" t="n"/>
+      <c r="P16" s="107" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q16" s="76" t="n"/>
-      <c r="R16" s="77" t="inlineStr">
+      <c r="Q16" s="105" t="n"/>
+      <c r="R16" s="106" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S16" s="79" t="inlineStr">
+      <c r="S16" s="108" t="inlineStr">
         <is>
           <t xml:space="preserve">5 pages </t>
         </is>
       </c>
-      <c r="T16" s="76" t="inlineStr">
+      <c r="T16" s="105" t="inlineStr">
         <is>
           <t>Box 8, Folder 6, Item 3</t>
         </is>
       </c>
-      <c r="U16" s="76" t="inlineStr">
+      <c r="U16" s="105" t="inlineStr">
         <is>
           <t>Glass Up. Use white paper as marker for section. Please make sure you scan complete section.</t>
         </is>
       </c>
-      <c r="V16" s="76" t="inlineStr">
+      <c r="V16" s="105" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F06.03</t>
         </is>
       </c>
-      <c r="W16" s="80" t="n">
+      <c r="W16" s="109" t="n">
         <v>45511</v>
       </c>
-      <c r="X16" s="79" t="inlineStr">
+      <c r="X16" s="108" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y16" s="76" t="n"/>
-      <c r="Z16" s="81" t="inlineStr">
+      <c r="Y16" s="105" t="n"/>
+      <c r="Z16" s="110" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA16" s="76" t="inlineStr">
+      <c r="AA16" s="105" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB16" s="76" t="inlineStr">
+      <c r="AB16" s="105" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC16" s="76" t="n"/>
-      <c r="AD16" s="76" t="n"/>
-      <c r="AE16" s="76" t="n"/>
-      <c r="AF16" s="76" t="n"/>
-      <c r="AG16" s="76" t="n"/>
+      <c r="AC16" s="105" t="n"/>
+      <c r="AD16" s="105" t="n"/>
+      <c r="AE16" s="105" t="n"/>
+      <c r="AF16" s="105" t="n"/>
+      <c r="AG16" s="105" t="n"/>
     </row>
     <row r="17" ht="15.75" customHeight="1" s="5">
-      <c r="A17" s="74" t="inlineStr">
+      <c r="A17" s="103" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B17" s="75" t="n">
+      <c r="B17" s="104" t="n">
         <v>13300</v>
       </c>
-      <c r="C17" s="76" t="n"/>
-      <c r="D17" s="76" t="n"/>
-      <c r="E17" s="76" t="n"/>
-      <c r="F17" s="77" t="inlineStr">
+      <c r="C17" s="105" t="n"/>
+      <c r="D17" s="105" t="n"/>
+      <c r="E17" s="105" t="n"/>
+      <c r="F17" s="106" t="inlineStr">
         <is>
           <t>William Stanley biography, early transcript draft with manuscript inserts</t>
         </is>
       </c>
-      <c r="G17" s="76" t="n"/>
-      <c r="H17" s="77" t="inlineStr">
+      <c r="G17" s="105" t="n"/>
+      <c r="H17" s="106" t="inlineStr">
         <is>
           <t>Author's Notes on "The Life of William Stanley" Trnascript by Thomas C. Martin</t>
         </is>
       </c>
-      <c r="I17" s="76" t="n"/>
-      <c r="J17" s="74" t="inlineStr">
+      <c r="I17" s="105" t="n"/>
+      <c r="J17" s="103" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="K17" s="74" t="inlineStr">
+      <c r="K17" s="103" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L17" s="76" t="n"/>
-      <c r="M17" s="74" t="inlineStr">
+      <c r="L17" s="105" t="n"/>
+      <c r="M17" s="103" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N17" s="76" t="n"/>
-      <c r="O17" s="76" t="n"/>
-      <c r="P17" s="78" t="inlineStr">
+      <c r="N17" s="105" t="n"/>
+      <c r="O17" s="105" t="n"/>
+      <c r="P17" s="107" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q17" s="76" t="n"/>
-      <c r="R17" s="77" t="inlineStr">
+      <c r="Q17" s="105" t="n"/>
+      <c r="R17" s="106" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S17" s="79" t="inlineStr">
+      <c r="S17" s="108" t="inlineStr">
         <is>
           <t xml:space="preserve">2 pages </t>
         </is>
       </c>
-      <c r="T17" s="76" t="inlineStr">
+      <c r="T17" s="105" t="inlineStr">
         <is>
           <t>Box 8, Folder 6, Item 4</t>
         </is>
       </c>
-      <c r="U17" s="76" t="inlineStr">
+      <c r="U17" s="105" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down. Remove plastic sleeve and replace carefully </t>
         </is>
       </c>
-      <c r="V17" s="76" t="inlineStr">
+      <c r="V17" s="105" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F06.04</t>
         </is>
       </c>
-      <c r="W17" s="80" t="n">
+      <c r="W17" s="109" t="n">
         <v>45511</v>
       </c>
-      <c r="X17" s="79" t="inlineStr">
+      <c r="X17" s="108" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y17" s="76" t="n"/>
-      <c r="Z17" s="81" t="inlineStr">
+      <c r="Y17" s="105" t="n"/>
+      <c r="Z17" s="110" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA17" s="76" t="inlineStr">
+      <c r="AA17" s="105" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB17" s="76" t="inlineStr">
+      <c r="AB17" s="105" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC17" s="76" t="n"/>
-      <c r="AD17" s="76" t="n"/>
-      <c r="AE17" s="76" t="n"/>
-      <c r="AF17" s="76" t="n"/>
-      <c r="AG17" s="76" t="n"/>
+      <c r="AC17" s="105" t="n"/>
+      <c r="AD17" s="105" t="n"/>
+      <c r="AE17" s="105" t="n"/>
+      <c r="AF17" s="105" t="n"/>
+      <c r="AG17" s="105" t="n"/>
     </row>
     <row r="18" ht="15.75" customHeight="1" s="5">
-      <c r="A18" s="74" t="inlineStr">
+      <c r="A18" s="103" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B18" s="75" t="n">
+      <c r="B18" s="104" t="n">
         <v>13300</v>
       </c>
-      <c r="C18" s="76" t="n"/>
-      <c r="D18" s="76" t="n"/>
-      <c r="E18" s="76" t="n"/>
-      <c r="F18" s="77" t="inlineStr">
+      <c r="C18" s="105" t="n"/>
+      <c r="D18" s="105" t="n"/>
+      <c r="E18" s="105" t="n"/>
+      <c r="F18" s="106" t="inlineStr">
         <is>
           <t>William Stanley biography, early transcript draft with manuscript inserts</t>
         </is>
       </c>
-      <c r="G18" s="76" t="n"/>
-      <c r="H18" s="77" t="inlineStr">
+      <c r="G18" s="105" t="n"/>
+      <c r="H18" s="106" t="inlineStr">
         <is>
           <t>Annotated Typescript Draft of "The Life of William Stanley" by Thomas C. Martin</t>
         </is>
       </c>
-      <c r="I18" s="76" t="inlineStr">
+      <c r="I18" s="105" t="inlineStr">
         <is>
           <t xml:space="preserve">Includes four drafts of Chapter 8. </t>
         </is>
       </c>
-      <c r="J18" s="74" t="inlineStr">
+      <c r="J18" s="103" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="K18" s="74" t="inlineStr">
+      <c r="K18" s="103" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L18" s="76" t="n"/>
-      <c r="M18" s="74" t="inlineStr">
+      <c r="L18" s="105" t="n"/>
+      <c r="M18" s="103" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N18" s="76" t="n"/>
-      <c r="O18" s="76" t="n"/>
-      <c r="P18" s="78" t="inlineStr">
+      <c r="N18" s="105" t="n"/>
+      <c r="O18" s="105" t="n"/>
+      <c r="P18" s="107" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q18" s="76" t="n"/>
-      <c r="R18" s="77" t="inlineStr">
+      <c r="Q18" s="105" t="n"/>
+      <c r="R18" s="106" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S18" s="79" t="inlineStr">
+      <c r="S18" s="108" t="inlineStr">
         <is>
           <t xml:space="preserve">154 pages </t>
         </is>
       </c>
-      <c r="T18" s="76" t="inlineStr">
+      <c r="T18" s="105" t="inlineStr">
         <is>
           <t>Box 8, Folder 6, Item 5</t>
         </is>
       </c>
-      <c r="U18" s="76" t="inlineStr">
+      <c r="U18" s="105" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down. Use caution to maintain orignal order. Some of the chapters are connected with plastic clips, please remove clips and do not replace them. </t>
         </is>
       </c>
-      <c r="V18" s="76" t="inlineStr">
+      <c r="V18" s="105" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F06.05</t>
         </is>
       </c>
-      <c r="W18" s="80" t="n">
+      <c r="W18" s="109" t="n">
         <v>45511</v>
       </c>
-      <c r="X18" s="79" t="inlineStr">
+      <c r="X18" s="108" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y18" s="76" t="n"/>
-      <c r="Z18" s="81" t="inlineStr">
+      <c r="Y18" s="105" t="n"/>
+      <c r="Z18" s="110" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA18" s="82" t="inlineStr">
+      <c r="AA18" s="111" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB18" s="76" t="inlineStr">
+      <c r="AB18" s="105" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC18" s="76" t="n"/>
-      <c r="AD18" s="76" t="n"/>
-      <c r="AE18" s="76" t="n"/>
-      <c r="AF18" s="76" t="n"/>
-      <c r="AG18" s="76" t="n"/>
+      <c r="AC18" s="105" t="n"/>
+      <c r="AD18" s="105" t="n"/>
+      <c r="AE18" s="105" t="n"/>
+      <c r="AF18" s="105" t="n"/>
+      <c r="AG18" s="105" t="n"/>
     </row>
     <row r="19" ht="15.75" customHeight="1" s="5">
-      <c r="A19" s="74" t="inlineStr">
+      <c r="A19" s="103" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B19" s="75" t="n">
+      <c r="B19" s="104" t="n">
         <v>13301</v>
       </c>
-      <c r="C19" s="76" t="n"/>
-      <c r="D19" s="76" t="n"/>
-      <c r="E19" s="76" t="n"/>
-      <c r="F19" s="77" t="inlineStr">
+      <c r="C19" s="105" t="n"/>
+      <c r="D19" s="105" t="n"/>
+      <c r="E19" s="105" t="n"/>
+      <c r="F19" s="106" t="inlineStr">
         <is>
           <t>William Stanley biography, printers typescript</t>
         </is>
       </c>
-      <c r="G19" s="76" t="n"/>
-      <c r="H19" s="77" t="inlineStr">
+      <c r="G19" s="105" t="n"/>
+      <c r="H19" s="106" t="inlineStr">
         <is>
           <t xml:space="preserve">Printer's Typewritten Text of "The Life of William Stanley" by Thomas C. Martin with Handwritten Notes </t>
         </is>
       </c>
-      <c r="I19" s="76" t="n"/>
-      <c r="J19" s="74" t="inlineStr">
+      <c r="I19" s="105" t="n"/>
+      <c r="J19" s="103" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="K19" s="74" t="inlineStr">
+      <c r="K19" s="103" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L19" s="76" t="n"/>
-      <c r="M19" s="74" t="inlineStr">
+      <c r="L19" s="105" t="n"/>
+      <c r="M19" s="103" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N19" s="76" t="n"/>
-      <c r="O19" s="76" t="n"/>
-      <c r="P19" s="78" t="inlineStr">
+      <c r="N19" s="105" t="n"/>
+      <c r="O19" s="105" t="n"/>
+      <c r="P19" s="107" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q19" s="76" t="n"/>
-      <c r="R19" s="77" t="inlineStr">
+      <c r="Q19" s="105" t="n"/>
+      <c r="R19" s="106" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S19" s="79" t="inlineStr">
+      <c r="S19" s="108" t="inlineStr">
         <is>
           <t xml:space="preserve">99 pages </t>
         </is>
       </c>
-      <c r="T19" s="76" t="inlineStr">
+      <c r="T19" s="105" t="inlineStr">
         <is>
           <t>Box 8, Folder 7</t>
         </is>
       </c>
-      <c r="U19" s="76" t="inlineStr">
+      <c r="U19" s="105" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Up, Paper is Extremely Brittle </t>
         </is>
       </c>
-      <c r="V19" s="76" t="inlineStr">
+      <c r="V19" s="105" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F07</t>
         </is>
       </c>
-      <c r="W19" s="83" t="n">
+      <c r="W19" s="112" t="n">
         <v>45511</v>
       </c>
-      <c r="X19" s="79" t="inlineStr">
+      <c r="X19" s="108" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
-      <c r="Y19" s="76" t="n"/>
-      <c r="Z19" s="81" t="inlineStr">
+      <c r="Y19" s="105" t="n"/>
+      <c r="Z19" s="110" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA19" s="76" t="inlineStr">
+      <c r="AA19" s="105" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB19" s="76" t="inlineStr">
+      <c r="AB19" s="105" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC19" s="76" t="n"/>
-      <c r="AD19" s="76" t="n"/>
-      <c r="AE19" s="76" t="n"/>
-      <c r="AF19" s="76" t="n"/>
-      <c r="AG19" s="76" t="n"/>
+      <c r="AC19" s="105" t="n"/>
+      <c r="AD19" s="105" t="n"/>
+      <c r="AE19" s="105" t="n"/>
+      <c r="AF19" s="105" t="n"/>
+      <c r="AG19" s="105" t="n"/>
     </row>
     <row r="20" ht="15.75" customHeight="1" s="5">
-      <c r="A20" s="74" t="inlineStr">
+      <c r="A20" s="103" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B20" s="75" t="n">
+      <c r="B20" s="104" t="n">
         <v>13339</v>
       </c>
-      <c r="C20" s="76" t="n"/>
-      <c r="D20" s="76" t="n"/>
-      <c r="E20" s="76" t="n"/>
-      <c r="F20" s="77" t="inlineStr">
+      <c r="C20" s="105" t="n"/>
+      <c r="D20" s="105" t="n"/>
+      <c r="E20" s="105" t="n"/>
+      <c r="F20" s="106" t="inlineStr">
         <is>
           <t>"Associations with William Stanley," typescripts</t>
         </is>
       </c>
-      <c r="G20" s="76" t="n"/>
-      <c r="H20" s="77" t="inlineStr">
+      <c r="G20" s="105" t="n"/>
+      <c r="H20" s="106" t="inlineStr">
         <is>
           <t xml:space="preserve">Typescript Draft of "Associates with William Stanley" by Cummings C. Chesney, Including "Play Ball" </t>
         </is>
       </c>
-      <c r="I20" s="76" t="n"/>
-      <c r="J20" s="74" t="inlineStr">
+      <c r="I20" s="105" t="n"/>
+      <c r="J20" s="103" t="inlineStr">
         <is>
           <t>Chesney, Cummings C.</t>
         </is>
       </c>
-      <c r="K20" s="74" t="inlineStr">
+      <c r="K20" s="103" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L20" s="76" t="n"/>
-      <c r="M20" s="74" t="inlineStr">
+      <c r="L20" s="105" t="n"/>
+      <c r="M20" s="103" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N20" s="76" t="n"/>
-      <c r="O20" s="76" t="n"/>
-      <c r="P20" s="78" t="inlineStr">
+      <c r="N20" s="105" t="n"/>
+      <c r="O20" s="105" t="n"/>
+      <c r="P20" s="107" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q20" s="76" t="n"/>
-      <c r="R20" s="77" t="inlineStr">
+      <c r="Q20" s="105" t="n"/>
+      <c r="R20" s="106" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S20" s="79" t="inlineStr">
+      <c r="S20" s="108" t="inlineStr">
         <is>
           <t xml:space="preserve">17 pages </t>
         </is>
       </c>
-      <c r="T20" s="76" t="inlineStr">
+      <c r="T20" s="105" t="inlineStr">
         <is>
           <t xml:space="preserve">Box 8, Folder 8, Item 1 </t>
         </is>
       </c>
-      <c r="U20" s="76" t="inlineStr">
+      <c r="U20" s="105" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down. </t>
         </is>
       </c>
-      <c r="V20" s="76" t="inlineStr">
+      <c r="V20" s="105" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F08.01</t>
         </is>
       </c>
-      <c r="W20" s="83" t="n">
+      <c r="W20" s="112" t="n">
         <v>45511</v>
       </c>
-      <c r="X20" s="76" t="inlineStr">
+      <c r="X20" s="105" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
-      <c r="Y20" s="76" t="n"/>
-      <c r="Z20" s="81" t="inlineStr">
+      <c r="Y20" s="105" t="n"/>
+      <c r="Z20" s="110" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA20" s="76" t="inlineStr">
+      <c r="AA20" s="105" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB20" s="76" t="inlineStr">
+      <c r="AB20" s="105" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC20" s="76" t="n"/>
-      <c r="AD20" s="76" t="n"/>
-      <c r="AE20" s="76" t="n"/>
-      <c r="AF20" s="76" t="n"/>
-      <c r="AG20" s="76" t="n"/>
+      <c r="AC20" s="105" t="n"/>
+      <c r="AD20" s="105" t="n"/>
+      <c r="AE20" s="105" t="n"/>
+      <c r="AF20" s="105" t="n"/>
+      <c r="AG20" s="105" t="n"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="5">
-      <c r="A21" s="74" t="inlineStr">
+      <c r="A21" s="103" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B21" s="75" t="n">
+      <c r="B21" s="104" t="n">
         <v>13339</v>
       </c>
-      <c r="C21" s="76" t="n"/>
-      <c r="D21" s="76" t="n"/>
-      <c r="E21" s="76" t="n"/>
-      <c r="F21" s="77" t="inlineStr">
+      <c r="C21" s="105" t="n"/>
+      <c r="D21" s="105" t="n"/>
+      <c r="E21" s="105" t="n"/>
+      <c r="F21" s="106" t="inlineStr">
         <is>
           <t>"Associations with William Stanley," typescripts</t>
         </is>
       </c>
-      <c r="G21" s="76" t="n"/>
-      <c r="H21" s="77" t="inlineStr">
+      <c r="G21" s="105" t="n"/>
+      <c r="H21" s="106" t="inlineStr">
         <is>
           <t xml:space="preserve">Typescript Draft of "Associates with William Stanley" by Cummings C. Chesney, Untitled </t>
         </is>
       </c>
-      <c r="I21" s="76" t="n"/>
-      <c r="J21" s="74" t="inlineStr">
+      <c r="I21" s="105" t="n"/>
+      <c r="J21" s="103" t="inlineStr">
         <is>
           <t>Chesney, Cummings C.</t>
         </is>
       </c>
-      <c r="K21" s="74" t="inlineStr">
+      <c r="K21" s="103" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L21" s="76" t="n"/>
-      <c r="M21" s="74" t="inlineStr">
+      <c r="L21" s="105" t="n"/>
+      <c r="M21" s="103" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N21" s="76" t="n"/>
-      <c r="O21" s="76" t="n"/>
-      <c r="P21" s="78" t="inlineStr">
+      <c r="N21" s="105" t="n"/>
+      <c r="O21" s="105" t="n"/>
+      <c r="P21" s="107" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q21" s="76" t="n"/>
-      <c r="R21" s="77" t="inlineStr">
+      <c r="Q21" s="105" t="n"/>
+      <c r="R21" s="106" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S21" s="79" t="inlineStr">
+      <c r="S21" s="108" t="inlineStr">
         <is>
           <t xml:space="preserve">13 pages </t>
         </is>
       </c>
-      <c r="T21" s="76" t="inlineStr">
+      <c r="T21" s="105" t="inlineStr">
         <is>
           <t>Box 8, Folder 8, Item 2</t>
         </is>
       </c>
-      <c r="U21" s="76" t="inlineStr">
+      <c r="U21" s="105" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down. </t>
         </is>
       </c>
-      <c r="V21" s="76" t="inlineStr">
+      <c r="V21" s="105" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F08.02</t>
         </is>
       </c>
-      <c r="W21" s="80" t="n">
+      <c r="W21" s="109" t="n">
         <v>45511</v>
       </c>
-      <c r="X21" s="76" t="inlineStr">
+      <c r="X21" s="105" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
-      <c r="Y21" s="76" t="n"/>
-      <c r="Z21" s="81" t="inlineStr">
+      <c r="Y21" s="105" t="n"/>
+      <c r="Z21" s="110" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA21" s="76" t="inlineStr">
+      <c r="AA21" s="105" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB21" s="76" t="inlineStr">
+      <c r="AB21" s="105" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC21" s="76" t="n"/>
-      <c r="AD21" s="76" t="n"/>
-      <c r="AE21" s="76" t="n"/>
-      <c r="AF21" s="76" t="n"/>
-      <c r="AG21" s="76" t="n"/>
+      <c r="AC21" s="105" t="n"/>
+      <c r="AD21" s="105" t="n"/>
+      <c r="AE21" s="105" t="n"/>
+      <c r="AF21" s="105" t="n"/>
+      <c r="AG21" s="105" t="n"/>
     </row>
     <row r="22" ht="15.75" customHeight="1" s="5">
-      <c r="A22" s="74" t="inlineStr">
+      <c r="A22" s="103" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B22" s="75" t="n">
+      <c r="B22" s="104" t="n">
         <v>13339</v>
       </c>
-      <c r="C22" s="76" t="n"/>
-      <c r="D22" s="76" t="n"/>
-      <c r="E22" s="76" t="n"/>
-      <c r="F22" s="77" t="inlineStr">
+      <c r="C22" s="105" t="n"/>
+      <c r="D22" s="105" t="n"/>
+      <c r="E22" s="105" t="n"/>
+      <c r="F22" s="106" t="inlineStr">
         <is>
           <t>"Associations with William Stanley," typescripts</t>
         </is>
       </c>
-      <c r="G22" s="76" t="n"/>
-      <c r="H22" s="77" t="inlineStr">
+      <c r="G22" s="105" t="n"/>
+      <c r="H22" s="106" t="inlineStr">
         <is>
           <t xml:space="preserve">Typescript Draft of "Associates with William Stanley" by Cummings C. Chesney, Untitled from Scientific and Industrial Information Bureau </t>
         </is>
       </c>
-      <c r="I22" s="76" t="n"/>
-      <c r="J22" s="74" t="inlineStr">
+      <c r="I22" s="105" t="n"/>
+      <c r="J22" s="103" t="inlineStr">
         <is>
           <t>Chesney, Cummings C.</t>
         </is>
       </c>
-      <c r="K22" s="74" t="inlineStr">
+      <c r="K22" s="103" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L22" s="76" t="n"/>
-      <c r="M22" s="74" t="inlineStr">
+      <c r="L22" s="105" t="n"/>
+      <c r="M22" s="103" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N22" s="76" t="n"/>
-      <c r="O22" s="76" t="n"/>
-      <c r="P22" s="78" t="inlineStr">
+      <c r="N22" s="105" t="n"/>
+      <c r="O22" s="105" t="n"/>
+      <c r="P22" s="107" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q22" s="76" t="n"/>
-      <c r="R22" s="77" t="inlineStr">
+      <c r="Q22" s="105" t="n"/>
+      <c r="R22" s="106" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S22" s="79" t="inlineStr">
+      <c r="S22" s="108" t="inlineStr">
         <is>
           <t xml:space="preserve">30 pages </t>
         </is>
       </c>
-      <c r="T22" s="76" t="inlineStr">
+      <c r="T22" s="105" t="inlineStr">
         <is>
           <t>Box 8, Folder 8, Item 3</t>
         </is>
       </c>
-      <c r="U22" s="76" t="inlineStr">
+      <c r="U22" s="105" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down. </t>
         </is>
       </c>
-      <c r="V22" s="76" t="inlineStr">
+      <c r="V22" s="105" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F08.03</t>
         </is>
       </c>
-      <c r="W22" s="80" t="n">
+      <c r="W22" s="109" t="n">
         <v>45511</v>
       </c>
-      <c r="X22" s="76" t="inlineStr">
+      <c r="X22" s="105" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
-      <c r="Y22" s="76" t="n"/>
-      <c r="Z22" s="81" t="inlineStr">
+      <c r="Y22" s="105" t="n"/>
+      <c r="Z22" s="110" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA22" s="76" t="inlineStr">
+      <c r="AA22" s="105" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB22" s="76" t="inlineStr">
+      <c r="AB22" s="105" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC22" s="76" t="n"/>
-      <c r="AD22" s="76" t="n"/>
-      <c r="AE22" s="76" t="n"/>
-      <c r="AF22" s="76" t="n"/>
-      <c r="AG22" s="76" t="n"/>
+      <c r="AC22" s="105" t="n"/>
+      <c r="AD22" s="105" t="n"/>
+      <c r="AE22" s="105" t="n"/>
+      <c r="AF22" s="105" t="n"/>
+      <c r="AG22" s="105" t="n"/>
     </row>
     <row r="23" ht="12.75" customHeight="1" s="5">
       <c r="P23" s="38" t="n"/>
@@ -7798,91 +7856,105 @@
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1" s="5">
-      <c r="A13" s="6" t="inlineStr">
+      <c r="A13" s="28" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B13" s="7" t="n">
+      <c r="B13" s="29" t="n">
         <v>13341</v>
       </c>
-      <c r="C13" s="6" t="n"/>
-      <c r="D13" s="6" t="n"/>
-      <c r="E13" s="6" t="n"/>
-      <c r="F13" s="6" t="inlineStr">
+      <c r="C13" s="28" t="n"/>
+      <c r="D13" s="28" t="n"/>
+      <c r="E13" s="28" t="n"/>
+      <c r="F13" s="28" t="inlineStr">
         <is>
           <t>Correspondence regarding National Cyclopedia of American Biography entry on William Stanley</t>
         </is>
       </c>
-      <c r="H13" s="9" t="inlineStr">
+      <c r="G13" s="30" t="n"/>
+      <c r="H13" s="31" t="inlineStr">
         <is>
           <t>Envelope addressed to Dr. Samuel A. Eliot, Editor-in-chief, Biographical History of Massachusetts</t>
         </is>
       </c>
-      <c r="J13" s="9" t="inlineStr">
+      <c r="I13" s="30" t="n"/>
+      <c r="J13" s="31" t="inlineStr">
         <is>
           <t>unknown</t>
         </is>
       </c>
-      <c r="N13" s="6" t="inlineStr">
+      <c r="K13" s="30" t="n"/>
+      <c r="L13" s="30" t="n"/>
+      <c r="M13" s="30" t="n"/>
+      <c r="N13" s="28" t="inlineStr">
         <is>
           <t>Stanley, William, 1858-1916</t>
         </is>
       </c>
-      <c r="P13" s="9" t="inlineStr">
+      <c r="O13" s="30" t="n"/>
+      <c r="P13" s="31" t="inlineStr">
         <is>
           <t>1909-1940</t>
         </is>
       </c>
-      <c r="Q13" s="38" t="n"/>
-      <c r="S13" s="9" t="inlineStr">
+      <c r="Q13" s="43" t="n"/>
+      <c r="R13" s="30" t="n"/>
+      <c r="S13" s="31" t="inlineStr">
         <is>
           <t>No Copyright - United States</t>
         </is>
       </c>
-      <c r="T13" s="9" t="inlineStr">
+      <c r="T13" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">5 pages </t>
         </is>
       </c>
-      <c r="U13" s="6" t="inlineStr">
+      <c r="U13" s="28" t="inlineStr">
         <is>
           <t>Box 9, Folder 2, Item 6</t>
         </is>
       </c>
-      <c r="V13" s="8" t="inlineStr">
+      <c r="V13" s="33" t="inlineStr">
         <is>
           <t>Glass down</t>
         </is>
       </c>
-      <c r="W13" s="9" t="inlineStr">
+      <c r="W13" s="31" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B09.F02.06</t>
         </is>
       </c>
-      <c r="X13" s="16" t="n">
+      <c r="X13" s="34" t="n">
         <v>45513</v>
       </c>
-      <c r="Y13" s="9" t="inlineStr">
+      <c r="Y13" s="31" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="AA13" s="6" t="inlineStr">
+      <c r="Z13" s="30" t="n"/>
+      <c r="AA13" s="28" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AB13" t="inlineStr">
+      <c r="AB13" s="30" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AC13" t="inlineStr">
+      <c r="AC13" s="30" t="inlineStr">
         <is>
           <t>Incorrect page count</t>
         </is>
       </c>
+      <c r="AD13" s="30" t="n"/>
+      <c r="AE13" s="30" t="n"/>
+      <c r="AF13" s="30" t="n"/>
+      <c r="AG13" s="30" t="n"/>
+      <c r="AH13" s="30" t="n"/>
+      <c r="AI13" s="30" t="n"/>
     </row>
     <row r="14" ht="15.75" customHeight="1" s="5">
       <c r="A14" s="6" t="inlineStr">
@@ -9207,84 +9279,101 @@
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1" s="5">
-      <c r="A30" s="6" t="inlineStr">
+      <c r="A30" s="28" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B30" s="7" t="n">
+      <c r="B30" s="29" t="n">
         <v>13341</v>
       </c>
-      <c r="F30" s="6" t="inlineStr">
+      <c r="C30" s="30" t="n"/>
+      <c r="D30" s="30" t="n"/>
+      <c r="E30" s="30" t="n"/>
+      <c r="F30" s="28" t="inlineStr">
         <is>
           <t>Correspondence regarding National Cyclopedia of American Biography entry on William Stanley</t>
         </is>
       </c>
-      <c r="H30" s="9" t="inlineStr">
+      <c r="G30" s="30" t="n"/>
+      <c r="H30" s="31" t="inlineStr">
         <is>
           <t>American Inventors pamphlet</t>
         </is>
       </c>
-      <c r="J30" s="9" t="inlineStr">
+      <c r="I30" s="30" t="n"/>
+      <c r="J30" s="31" t="inlineStr">
         <is>
           <t>The National Cyclopedia of American Biography</t>
         </is>
       </c>
-      <c r="N30" s="6" t="inlineStr">
+      <c r="K30" s="30" t="n"/>
+      <c r="L30" s="30" t="n"/>
+      <c r="M30" s="30" t="n"/>
+      <c r="N30" s="28" t="inlineStr">
         <is>
           <t>Stanley, William, 1858-1916</t>
         </is>
       </c>
-      <c r="P30" s="9" t="inlineStr">
+      <c r="O30" s="30" t="n"/>
+      <c r="P30" s="31" t="inlineStr">
         <is>
           <t>1910-1920</t>
         </is>
       </c>
-      <c r="Q30" s="38" t="n"/>
-      <c r="S30" s="9" t="inlineStr">
+      <c r="Q30" s="43" t="n"/>
+      <c r="R30" s="30" t="n"/>
+      <c r="S30" s="31" t="inlineStr">
         <is>
           <t>Copyright Undetermined</t>
         </is>
       </c>
-      <c r="T30" s="9" t="n"/>
-      <c r="U30" s="6" t="inlineStr">
+      <c r="T30" s="31" t="n"/>
+      <c r="U30" s="28" t="inlineStr">
         <is>
           <t>Box 9, Folder 2, Item 23</t>
         </is>
       </c>
-      <c r="V30" s="8" t="inlineStr">
+      <c r="V30" s="33" t="inlineStr">
         <is>
           <t>Glass down</t>
         </is>
       </c>
-      <c r="W30" s="9" t="inlineStr">
+      <c r="W30" s="31" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B09.F02.23</t>
         </is>
       </c>
-      <c r="X30" s="16" t="n">
+      <c r="X30" s="34" t="n">
         <v>45513</v>
       </c>
-      <c r="Y30" s="9" t="inlineStr">
+      <c r="Y30" s="31" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="AA30" s="6" t="inlineStr">
+      <c r="Z30" s="30" t="n"/>
+      <c r="AA30" s="28" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AB30" t="inlineStr">
+      <c r="AB30" s="30" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AC30" t="inlineStr">
+      <c r="AC30" s="30" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
+      <c r="AD30" s="30" t="n"/>
+      <c r="AE30" s="30" t="n"/>
+      <c r="AF30" s="30" t="n"/>
+      <c r="AG30" s="30" t="n"/>
+      <c r="AH30" s="30" t="n"/>
+      <c r="AI30" s="30" t="n"/>
     </row>
     <row r="31" ht="15.75" customHeight="1" s="5">
       <c r="A31" s="6" t="inlineStr">
@@ -16838,88 +16927,105 @@
       </c>
     </row>
     <row r="122" ht="15" customHeight="1" s="5">
-      <c r="A122" s="6" t="inlineStr">
+      <c r="A122" s="28" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B122" s="7" t="n">
+      <c r="B122" s="29" t="n">
         <v>13344</v>
       </c>
-      <c r="F122" s="6" t="inlineStr">
+      <c r="C122" s="30" t="n"/>
+      <c r="D122" s="30" t="n"/>
+      <c r="E122" s="30" t="n"/>
+      <c r="F122" s="28" t="inlineStr">
         <is>
           <t>Correspondence regarding William Stanley biography</t>
         </is>
       </c>
-      <c r="H122" s="9" t="inlineStr">
+      <c r="G122" s="30" t="n"/>
+      <c r="H122" s="31" t="inlineStr">
         <is>
           <t>Table of contents draft for Life of William Stanley manuscript</t>
         </is>
       </c>
-      <c r="J122" s="9" t="inlineStr">
+      <c r="I122" s="30" t="n"/>
+      <c r="J122" s="31" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="N122" s="9" t="inlineStr">
+      <c r="K122" s="30" t="n"/>
+      <c r="L122" s="30" t="n"/>
+      <c r="M122" s="30" t="n"/>
+      <c r="N122" s="31" t="inlineStr">
         <is>
           <t>Stanley, William, 1858-1916</t>
         </is>
       </c>
-      <c r="P122" s="9" t="inlineStr">
+      <c r="O122" s="30" t="n"/>
+      <c r="P122" s="31" t="inlineStr">
         <is>
           <t>1922-1924</t>
         </is>
       </c>
-      <c r="Q122" s="38" t="n"/>
-      <c r="S122" s="9" t="inlineStr">
+      <c r="Q122" s="43" t="n"/>
+      <c r="R122" s="30" t="n"/>
+      <c r="S122" s="31" t="inlineStr">
         <is>
           <t>No Copyright - United States</t>
         </is>
       </c>
-      <c r="T122" s="9" t="inlineStr">
+      <c r="T122" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">1 page </t>
         </is>
       </c>
-      <c r="U122" s="6" t="inlineStr">
+      <c r="U122" s="28" t="inlineStr">
         <is>
           <t>Box 9, Folder 5, Item 67</t>
         </is>
       </c>
-      <c r="V122" s="8" t="inlineStr">
+      <c r="V122" s="33" t="inlineStr">
         <is>
           <t>Glass down</t>
         </is>
       </c>
-      <c r="W122" s="9" t="inlineStr">
+      <c r="W122" s="31" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B09.F05.67</t>
         </is>
       </c>
-      <c r="X122" s="16" t="n">
+      <c r="X122" s="34" t="n">
         <v>45523</v>
       </c>
-      <c r="Y122" s="9" t="inlineStr">
+      <c r="Y122" s="31" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="AA122" s="6" t="inlineStr">
+      <c r="Z122" s="30" t="n"/>
+      <c r="AA122" s="28" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AB122" t="inlineStr">
+      <c r="AB122" s="30" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AC122" t="inlineStr">
+      <c r="AC122" s="30" t="inlineStr">
         <is>
           <t>Incorrect page count</t>
         </is>
       </c>
+      <c r="AD122" s="30" t="n"/>
+      <c r="AE122" s="30" t="n"/>
+      <c r="AF122" s="30" t="n"/>
+      <c r="AG122" s="30" t="n"/>
+      <c r="AH122" s="30" t="n"/>
+      <c r="AI122" s="30" t="n"/>
     </row>
     <row r="123" ht="15" customHeight="1" s="5">
       <c r="A123" s="6" t="inlineStr">
@@ -17977,105 +18083,105 @@
       </c>
     </row>
     <row r="136" ht="15" customHeight="1" s="5">
-      <c r="A136" s="81" t="inlineStr">
+      <c r="A136" s="110" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B136" s="84" t="n">
+      <c r="B136" s="113" t="n">
         <v>13344</v>
       </c>
-      <c r="C136" s="81" t="n"/>
-      <c r="D136" s="81" t="n"/>
-      <c r="E136" s="81" t="n"/>
-      <c r="F136" s="81" t="inlineStr">
+      <c r="C136" s="110" t="n"/>
+      <c r="D136" s="110" t="n"/>
+      <c r="E136" s="110" t="n"/>
+      <c r="F136" s="110" t="inlineStr">
         <is>
           <t>Correspondence regarding William Stanley biography</t>
         </is>
       </c>
-      <c r="G136" s="85" t="n"/>
-      <c r="H136" s="79" t="inlineStr">
+      <c r="G136" s="114" t="n"/>
+      <c r="H136" s="108" t="inlineStr">
         <is>
           <t>Letter from C. C. Chesney to T. C. Martin, November 13, 1922, with enclosures</t>
         </is>
       </c>
-      <c r="I136" s="79" t="inlineStr">
+      <c r="I136" s="108" t="inlineStr">
         <is>
           <t>Enclosures: Letter from F. Darlington to T. C. Martin, November 5, 1922 and letter from  Philip G. Gossler to T. C. Martin, November 6, 1922</t>
         </is>
       </c>
-      <c r="J136" s="79" t="inlineStr">
+      <c r="J136" s="108" t="inlineStr">
         <is>
           <t>Chesney, Cummings C.;Darlington, Frederick;Gossler, Philip G.</t>
         </is>
       </c>
-      <c r="K136" s="85" t="n"/>
-      <c r="L136" s="85" t="n"/>
-      <c r="M136" s="85" t="n"/>
-      <c r="N136" s="79" t="inlineStr">
+      <c r="K136" s="114" t="n"/>
+      <c r="L136" s="114" t="n"/>
+      <c r="M136" s="114" t="n"/>
+      <c r="N136" s="108" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924;Stanley, William, 1858-1916</t>
         </is>
       </c>
-      <c r="O136" s="85" t="n"/>
-      <c r="P136" s="85" t="n"/>
-      <c r="Q136" s="86" t="inlineStr">
+      <c r="O136" s="114" t="n"/>
+      <c r="P136" s="114" t="n"/>
+      <c r="Q136" s="115" t="inlineStr">
         <is>
           <t>1922-11-06;1922-11-08;1922-11-13</t>
         </is>
       </c>
-      <c r="R136" s="85" t="n"/>
-      <c r="S136" s="79" t="inlineStr">
+      <c r="R136" s="114" t="n"/>
+      <c r="S136" s="108" t="inlineStr">
         <is>
           <t>No Copyright - United States</t>
         </is>
       </c>
-      <c r="T136" s="85" t="n"/>
-      <c r="U136" s="81" t="inlineStr">
+      <c r="T136" s="114" t="n"/>
+      <c r="U136" s="110" t="inlineStr">
         <is>
           <t>Box 9, Folder 5, Item 81</t>
         </is>
       </c>
-      <c r="V136" s="87" t="inlineStr">
+      <c r="V136" s="116" t="inlineStr">
         <is>
           <t>Glass down</t>
         </is>
       </c>
-      <c r="W136" s="79" t="inlineStr">
+      <c r="W136" s="108" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B09.F05.81</t>
         </is>
       </c>
-      <c r="X136" s="88" t="n">
+      <c r="X136" s="117" t="n">
         <v>45523</v>
       </c>
-      <c r="Y136" s="79" t="inlineStr">
+      <c r="Y136" s="108" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Z136" s="85" t="n"/>
-      <c r="AA136" s="81" t="inlineStr">
+      <c r="Z136" s="114" t="n"/>
+      <c r="AA136" s="110" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AB136" s="85" t="inlineStr">
+      <c r="AB136" s="114" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AC136" s="85" t="inlineStr">
+      <c r="AC136" s="114" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AD136" s="85" t="n"/>
-      <c r="AE136" s="85" t="n"/>
-      <c r="AF136" s="85" t="n"/>
-      <c r="AG136" s="85" t="n"/>
-      <c r="AH136" s="85" t="n"/>
-      <c r="AI136" s="85" t="n"/>
+      <c r="AD136" s="114" t="n"/>
+      <c r="AE136" s="114" t="n"/>
+      <c r="AF136" s="114" t="n"/>
+      <c r="AG136" s="114" t="n"/>
+      <c r="AH136" s="114" t="n"/>
+      <c r="AI136" s="114" t="n"/>
     </row>
     <row r="137" ht="15" customHeight="1" s="5">
       <c r="A137" s="6" t="inlineStr">
@@ -18315,83 +18421,99 @@
       </c>
     </row>
     <row r="140" ht="15" customHeight="1" s="5">
-      <c r="A140" s="6" t="inlineStr">
+      <c r="A140" s="28" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B140" s="7" t="n">
+      <c r="B140" s="29" t="n">
         <v>13344</v>
       </c>
-      <c r="C140" s="6" t="n"/>
-      <c r="D140" s="6" t="n"/>
-      <c r="E140" s="6" t="n"/>
-      <c r="F140" s="6" t="inlineStr">
+      <c r="C140" s="28" t="n"/>
+      <c r="D140" s="28" t="n"/>
+      <c r="E140" s="28" t="n"/>
+      <c r="F140" s="28" t="inlineStr">
         <is>
           <t>Correspondence regarding William Stanley biography</t>
         </is>
       </c>
-      <c r="H140" s="9" t="inlineStr">
+      <c r="G140" s="30" t="n"/>
+      <c r="H140" s="31" t="inlineStr">
         <is>
           <t>Letter from [T. C. Martin] to C. C. Chesney, October 11, 1922</t>
         </is>
       </c>
-      <c r="J140" s="9" t="inlineStr">
+      <c r="I140" s="30" t="n"/>
+      <c r="J140" s="31" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="N140" s="9" t="inlineStr">
+      <c r="K140" s="30" t="n"/>
+      <c r="L140" s="30" t="n"/>
+      <c r="M140" s="30" t="n"/>
+      <c r="N140" s="31" t="inlineStr">
         <is>
           <t>Chesney, Cummings C.;Stanley, William, 1858-1916</t>
         </is>
       </c>
-      <c r="Q140" s="40" t="n">
+      <c r="O140" s="30" t="n"/>
+      <c r="P140" s="30" t="n"/>
+      <c r="Q140" s="44" t="n">
         <v>8320</v>
       </c>
-      <c r="S140" s="9" t="inlineStr">
+      <c r="R140" s="30" t="n"/>
+      <c r="S140" s="31" t="inlineStr">
         <is>
           <t>No Copyright - United States</t>
         </is>
       </c>
-      <c r="U140" s="6" t="inlineStr">
+      <c r="T140" s="30" t="n"/>
+      <c r="U140" s="28" t="inlineStr">
         <is>
           <t>Box 9, Folder 5, Item 85</t>
         </is>
       </c>
-      <c r="V140" s="8" t="inlineStr">
+      <c r="V140" s="33" t="inlineStr">
         <is>
           <t>Glass down</t>
         </is>
       </c>
-      <c r="W140" s="9" t="inlineStr">
+      <c r="W140" s="31" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B09.F05.85</t>
         </is>
       </c>
-      <c r="X140" s="16" t="n">
+      <c r="X140" s="34" t="n">
         <v>45523</v>
       </c>
-      <c r="Y140" s="9" t="inlineStr">
+      <c r="Y140" s="31" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="AA140" s="6" t="inlineStr">
+      <c r="Z140" s="30" t="n"/>
+      <c r="AA140" s="28" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AB140" t="inlineStr">
+      <c r="AB140" s="30" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AC140" t="inlineStr">
+      <c r="AC140" s="30" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
+      <c r="AD140" s="30" t="n"/>
+      <c r="AE140" s="30" t="n"/>
+      <c r="AF140" s="30" t="n"/>
+      <c r="AG140" s="30" t="n"/>
+      <c r="AH140" s="30" t="n"/>
+      <c r="AI140" s="30" t="n"/>
     </row>
     <row r="141" ht="15" customHeight="1" s="5">
       <c r="A141" s="6" t="inlineStr">
@@ -22917,101 +23039,101 @@
       </c>
     </row>
     <row r="198" ht="15" customHeight="1" s="5">
-      <c r="A198" s="81" t="inlineStr">
+      <c r="A198" s="110" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B198" s="84" t="n">
+      <c r="B198" s="113" t="n">
         <v>13346</v>
       </c>
-      <c r="C198" s="81" t="n"/>
-      <c r="D198" s="81" t="n"/>
-      <c r="E198" s="81" t="n"/>
-      <c r="F198" s="81" t="inlineStr">
+      <c r="C198" s="110" t="n"/>
+      <c r="D198" s="110" t="n"/>
+      <c r="E198" s="110" t="n"/>
+      <c r="F198" s="110" t="inlineStr">
         <is>
           <t>Biographical articles and brochures</t>
         </is>
       </c>
-      <c r="G198" s="85" t="n"/>
-      <c r="H198" s="81" t="inlineStr">
+      <c r="G198" s="114" t="n"/>
+      <c r="H198" s="110" t="inlineStr">
         <is>
           <t>Biographical articles and brochures, Item 9</t>
         </is>
       </c>
-      <c r="I198" s="85" t="n"/>
-      <c r="J198" s="79" t="inlineStr">
+      <c r="I198" s="114" t="n"/>
+      <c r="J198" s="108" t="inlineStr">
         <is>
           <t>unknown</t>
         </is>
       </c>
-      <c r="K198" s="85" t="n"/>
-      <c r="L198" s="85" t="n"/>
-      <c r="M198" s="85" t="n"/>
-      <c r="N198" s="79" t="inlineStr">
+      <c r="K198" s="114" t="n"/>
+      <c r="L198" s="114" t="n"/>
+      <c r="M198" s="114" t="n"/>
+      <c r="N198" s="108" t="inlineStr">
         <is>
           <t>Stanley, William, 1858-1916</t>
         </is>
       </c>
-      <c r="O198" s="85" t="n"/>
-      <c r="P198" s="85" t="n"/>
-      <c r="Q198" s="86" t="inlineStr">
+      <c r="O198" s="114" t="n"/>
+      <c r="P198" s="114" t="n"/>
+      <c r="Q198" s="115" t="inlineStr">
         <is>
           <t>unknown</t>
         </is>
       </c>
-      <c r="R198" s="85" t="n"/>
-      <c r="S198" s="79" t="inlineStr">
+      <c r="R198" s="114" t="n"/>
+      <c r="S198" s="108" t="inlineStr">
         <is>
           <t>Copyright Undetermined</t>
         </is>
       </c>
-      <c r="T198" s="85" t="n"/>
-      <c r="U198" s="79" t="inlineStr">
+      <c r="T198" s="114" t="n"/>
+      <c r="U198" s="108" t="inlineStr">
         <is>
           <t>Box 9, Folder 8, Item 9</t>
         </is>
       </c>
-      <c r="V198" s="87" t="inlineStr">
+      <c r="V198" s="116" t="inlineStr">
         <is>
           <t>Glass down</t>
         </is>
       </c>
-      <c r="W198" s="79" t="inlineStr">
+      <c r="W198" s="108" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B09.F08.09</t>
         </is>
       </c>
-      <c r="X198" s="88" t="n">
+      <c r="X198" s="117" t="n">
         <v>45524</v>
       </c>
-      <c r="Y198" s="79" t="inlineStr">
+      <c r="Y198" s="108" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Z198" s="85" t="n"/>
-      <c r="AA198" s="81" t="inlineStr">
+      <c r="Z198" s="114" t="n"/>
+      <c r="AA198" s="110" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AB198" s="85" t="inlineStr">
+      <c r="AB198" s="114" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AC198" s="85" t="inlineStr">
+      <c r="AC198" s="114" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AD198" s="85" t="n"/>
-      <c r="AE198" s="85" t="n"/>
-      <c r="AF198" s="85" t="n"/>
-      <c r="AG198" s="85" t="n"/>
-      <c r="AH198" s="85" t="n"/>
-      <c r="AI198" s="85" t="n"/>
+      <c r="AD198" s="114" t="n"/>
+      <c r="AE198" s="114" t="n"/>
+      <c r="AF198" s="114" t="n"/>
+      <c r="AG198" s="114" t="n"/>
+      <c r="AH198" s="114" t="n"/>
+      <c r="AI198" s="114" t="n"/>
     </row>
     <row r="199" ht="15" customHeight="1" s="5">
       <c r="A199" s="6" t="inlineStr">

</xml_diff>

<commit_message>
up-to-date spreadsheets' git push
</commit_message>
<xml_diff>
--- a/app/spreadsheets/sample.xlsx
+++ b/app/spreadsheets/sample.xlsx
@@ -1897,935 +1897,935 @@
       <c r="AG13" s="4" t="n"/>
     </row>
     <row r="14" ht="15.75" customHeight="1" s="5">
-      <c r="A14" s="103" t="inlineStr">
+      <c r="A14" s="1" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B14" s="104" t="n">
+      <c r="B14" s="11" t="n">
         <v>13300</v>
       </c>
-      <c r="C14" s="105" t="n"/>
-      <c r="D14" s="105" t="n"/>
-      <c r="E14" s="105" t="n"/>
-      <c r="F14" s="106" t="inlineStr">
+      <c r="C14" s="4" t="n"/>
+      <c r="D14" s="4" t="n"/>
+      <c r="E14" s="4" t="n"/>
+      <c r="F14" s="2" t="inlineStr">
         <is>
           <t>William Stanley biography, early transcript draft with manuscript inserts</t>
         </is>
       </c>
-      <c r="G14" s="105" t="n"/>
-      <c r="H14" s="106" t="inlineStr">
+      <c r="G14" s="4" t="n"/>
+      <c r="H14" s="2" t="inlineStr">
         <is>
           <t>Sections of Typescript Draft of "The Life of William Stanley" by Thomas C. Martin, "Stanley as Inventor and Manufacturer at Pittsfield"</t>
         </is>
       </c>
-      <c r="I14" s="105" t="n"/>
-      <c r="J14" s="103" t="inlineStr">
+      <c r="I14" s="4" t="n"/>
+      <c r="J14" s="1" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="K14" s="103" t="inlineStr">
+      <c r="K14" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L14" s="105" t="n"/>
-      <c r="M14" s="103" t="inlineStr">
+      <c r="L14" s="4" t="n"/>
+      <c r="M14" s="1" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N14" s="105" t="n"/>
-      <c r="O14" s="105" t="n"/>
-      <c r="P14" s="107" t="inlineStr">
+      <c r="N14" s="4" t="n"/>
+      <c r="O14" s="4" t="n"/>
+      <c r="P14" s="36" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q14" s="105" t="n"/>
-      <c r="R14" s="106" t="inlineStr">
+      <c r="Q14" s="4" t="n"/>
+      <c r="R14" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S14" s="108" t="inlineStr">
+      <c r="S14" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">14 pages </t>
         </is>
       </c>
-      <c r="T14" s="105" t="inlineStr">
+      <c r="T14" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">Box 8, Folder 6, Item 1  </t>
         </is>
       </c>
-      <c r="U14" s="105" t="inlineStr">
+      <c r="U14" s="4" t="inlineStr">
         <is>
           <t>Glass Down. Goes until Page 14. Please make sure you scan complete section.</t>
         </is>
       </c>
-      <c r="V14" s="105" t="inlineStr">
+      <c r="V14" s="4" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F06.01</t>
         </is>
       </c>
-      <c r="W14" s="109" t="n">
+      <c r="W14" s="15" t="n">
         <v>45510</v>
       </c>
-      <c r="X14" s="108" t="inlineStr">
+      <c r="X14" s="9" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y14" s="105" t="n"/>
-      <c r="Z14" s="110" t="inlineStr">
+      <c r="Y14" s="4" t="n"/>
+      <c r="Z14" s="6" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA14" s="105" t="inlineStr">
+      <c r="AA14" s="4" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB14" s="105" t="inlineStr">
+      <c r="AB14" s="4" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC14" s="105" t="n"/>
-      <c r="AD14" s="105" t="n"/>
-      <c r="AE14" s="105" t="n"/>
-      <c r="AF14" s="105" t="n"/>
-      <c r="AG14" s="105" t="n"/>
+      <c r="AC14" s="4" t="n"/>
+      <c r="AD14" s="4" t="n"/>
+      <c r="AE14" s="4" t="n"/>
+      <c r="AF14" s="4" t="n"/>
+      <c r="AG14" s="4" t="n"/>
     </row>
     <row r="15" ht="15.75" customHeight="1" s="5">
-      <c r="A15" s="103" t="inlineStr">
+      <c r="A15" s="1" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B15" s="104" t="n">
+      <c r="B15" s="11" t="n">
         <v>13300</v>
       </c>
-      <c r="C15" s="105" t="n"/>
-      <c r="D15" s="105" t="n"/>
-      <c r="E15" s="105" t="n"/>
-      <c r="F15" s="106" t="inlineStr">
+      <c r="C15" s="4" t="n"/>
+      <c r="D15" s="4" t="n"/>
+      <c r="E15" s="4" t="n"/>
+      <c r="F15" s="2" t="inlineStr">
         <is>
           <t>William Stanley biography, early transcript draft with manuscript inserts</t>
         </is>
       </c>
-      <c r="G15" s="105" t="n"/>
-      <c r="H15" s="106" t="inlineStr">
+      <c r="G15" s="4" t="n"/>
+      <c r="H15" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Sections of Typescript Draft of "The Life of William Stanley" by Thomas C. Martin, Untitiled from Scientific and Industrial Information Bureau </t>
         </is>
       </c>
-      <c r="I15" s="105" t="n"/>
-      <c r="J15" s="103" t="inlineStr">
+      <c r="I15" s="4" t="n"/>
+      <c r="J15" s="1" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="K15" s="103" t="inlineStr">
+      <c r="K15" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L15" s="105" t="n"/>
-      <c r="M15" s="103" t="inlineStr">
+      <c r="L15" s="4" t="n"/>
+      <c r="M15" s="1" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N15" s="105" t="n"/>
-      <c r="O15" s="105" t="n"/>
-      <c r="P15" s="107" t="inlineStr">
+      <c r="N15" s="4" t="n"/>
+      <c r="O15" s="4" t="n"/>
+      <c r="P15" s="36" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q15" s="105" t="n"/>
-      <c r="R15" s="106" t="inlineStr">
+      <c r="Q15" s="4" t="n"/>
+      <c r="R15" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S15" s="108" t="inlineStr">
+      <c r="S15" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">21 pages </t>
         </is>
       </c>
-      <c r="T15" s="105" t="inlineStr">
+      <c r="T15" s="4" t="inlineStr">
         <is>
           <t>Box 8, Folder 6, Item 2</t>
         </is>
       </c>
-      <c r="U15" s="105" t="inlineStr">
+      <c r="U15" s="4" t="inlineStr">
         <is>
           <t>Glass Down. Use white paper as marker for section. Please make sure you scan complete section.</t>
         </is>
       </c>
-      <c r="V15" s="105" t="inlineStr">
+      <c r="V15" s="4" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F06.02</t>
         </is>
       </c>
-      <c r="W15" s="109" t="n">
+      <c r="W15" s="15" t="n">
         <v>45511</v>
       </c>
-      <c r="X15" s="108" t="inlineStr">
+      <c r="X15" s="9" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y15" s="105" t="n"/>
-      <c r="Z15" s="110" t="inlineStr">
+      <c r="Y15" s="4" t="n"/>
+      <c r="Z15" s="6" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA15" s="105" t="inlineStr">
+      <c r="AA15" s="4" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB15" s="105" t="inlineStr">
+      <c r="AB15" s="4" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC15" s="105" t="n"/>
-      <c r="AD15" s="105" t="n"/>
-      <c r="AE15" s="105" t="n"/>
-      <c r="AF15" s="105" t="n"/>
-      <c r="AG15" s="105" t="n"/>
+      <c r="AC15" s="4" t="n"/>
+      <c r="AD15" s="4" t="n"/>
+      <c r="AE15" s="4" t="n"/>
+      <c r="AF15" s="4" t="n"/>
+      <c r="AG15" s="4" t="n"/>
     </row>
     <row r="16" ht="15.75" customHeight="1" s="5">
-      <c r="A16" s="103" t="inlineStr">
+      <c r="A16" s="1" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B16" s="104" t="n">
+      <c r="B16" s="11" t="n">
         <v>13300</v>
       </c>
-      <c r="C16" s="105" t="n"/>
-      <c r="D16" s="105" t="n"/>
-      <c r="E16" s="105" t="n"/>
-      <c r="F16" s="106" t="inlineStr">
+      <c r="C16" s="4" t="n"/>
+      <c r="D16" s="4" t="n"/>
+      <c r="E16" s="4" t="n"/>
+      <c r="F16" s="2" t="inlineStr">
         <is>
           <t>William Stanley biography, early transcript draft with manuscript inserts</t>
         </is>
       </c>
-      <c r="G16" s="105" t="n"/>
-      <c r="H16" s="106" t="inlineStr">
+      <c r="G16" s="4" t="n"/>
+      <c r="H16" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Sections of Typescript Draft of "The Life of William Stanley" by Thomas C. Martin, Untitiled </t>
         </is>
       </c>
-      <c r="I16" s="105" t="n"/>
-      <c r="J16" s="103" t="inlineStr">
+      <c r="I16" s="4" t="n"/>
+      <c r="J16" s="1" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="K16" s="103" t="inlineStr">
+      <c r="K16" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L16" s="105" t="n"/>
-      <c r="M16" s="103" t="inlineStr">
+      <c r="L16" s="4" t="n"/>
+      <c r="M16" s="1" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N16" s="105" t="n"/>
-      <c r="O16" s="105" t="n"/>
-      <c r="P16" s="107" t="inlineStr">
+      <c r="N16" s="4" t="n"/>
+      <c r="O16" s="4" t="n"/>
+      <c r="P16" s="36" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q16" s="105" t="n"/>
-      <c r="R16" s="106" t="inlineStr">
+      <c r="Q16" s="4" t="n"/>
+      <c r="R16" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S16" s="108" t="inlineStr">
+      <c r="S16" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">5 pages </t>
         </is>
       </c>
-      <c r="T16" s="105" t="inlineStr">
+      <c r="T16" s="4" t="inlineStr">
         <is>
           <t>Box 8, Folder 6, Item 3</t>
         </is>
       </c>
-      <c r="U16" s="105" t="inlineStr">
+      <c r="U16" s="4" t="inlineStr">
         <is>
           <t>Glass Up. Use white paper as marker for section. Please make sure you scan complete section.</t>
         </is>
       </c>
-      <c r="V16" s="105" t="inlineStr">
+      <c r="V16" s="4" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F06.03</t>
         </is>
       </c>
-      <c r="W16" s="109" t="n">
+      <c r="W16" s="15" t="n">
         <v>45511</v>
       </c>
-      <c r="X16" s="108" t="inlineStr">
+      <c r="X16" s="9" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y16" s="105" t="n"/>
-      <c r="Z16" s="110" t="inlineStr">
+      <c r="Y16" s="4" t="n"/>
+      <c r="Z16" s="6" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA16" s="105" t="inlineStr">
+      <c r="AA16" s="4" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB16" s="105" t="inlineStr">
+      <c r="AB16" s="4" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC16" s="105" t="n"/>
-      <c r="AD16" s="105" t="n"/>
-      <c r="AE16" s="105" t="n"/>
-      <c r="AF16" s="105" t="n"/>
-      <c r="AG16" s="105" t="n"/>
+      <c r="AC16" s="4" t="n"/>
+      <c r="AD16" s="4" t="n"/>
+      <c r="AE16" s="4" t="n"/>
+      <c r="AF16" s="4" t="n"/>
+      <c r="AG16" s="4" t="n"/>
     </row>
     <row r="17" ht="15.75" customHeight="1" s="5">
-      <c r="A17" s="103" t="inlineStr">
+      <c r="A17" s="1" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B17" s="104" t="n">
+      <c r="B17" s="11" t="n">
         <v>13300</v>
       </c>
-      <c r="C17" s="105" t="n"/>
-      <c r="D17" s="105" t="n"/>
-      <c r="E17" s="105" t="n"/>
-      <c r="F17" s="106" t="inlineStr">
+      <c r="C17" s="4" t="n"/>
+      <c r="D17" s="4" t="n"/>
+      <c r="E17" s="4" t="n"/>
+      <c r="F17" s="2" t="inlineStr">
         <is>
           <t>William Stanley biography, early transcript draft with manuscript inserts</t>
         </is>
       </c>
-      <c r="G17" s="105" t="n"/>
-      <c r="H17" s="106" t="inlineStr">
+      <c r="G17" s="4" t="n"/>
+      <c r="H17" s="2" t="inlineStr">
         <is>
           <t>Author's Notes on "The Life of William Stanley" Trnascript by Thomas C. Martin</t>
         </is>
       </c>
-      <c r="I17" s="105" t="n"/>
-      <c r="J17" s="103" t="inlineStr">
+      <c r="I17" s="4" t="n"/>
+      <c r="J17" s="1" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="K17" s="103" t="inlineStr">
+      <c r="K17" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L17" s="105" t="n"/>
-      <c r="M17" s="103" t="inlineStr">
+      <c r="L17" s="4" t="n"/>
+      <c r="M17" s="1" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N17" s="105" t="n"/>
-      <c r="O17" s="105" t="n"/>
-      <c r="P17" s="107" t="inlineStr">
+      <c r="N17" s="4" t="n"/>
+      <c r="O17" s="4" t="n"/>
+      <c r="P17" s="36" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q17" s="105" t="n"/>
-      <c r="R17" s="106" t="inlineStr">
+      <c r="Q17" s="4" t="n"/>
+      <c r="R17" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S17" s="108" t="inlineStr">
+      <c r="S17" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">2 pages </t>
         </is>
       </c>
-      <c r="T17" s="105" t="inlineStr">
+      <c r="T17" s="4" t="inlineStr">
         <is>
           <t>Box 8, Folder 6, Item 4</t>
         </is>
       </c>
-      <c r="U17" s="105" t="inlineStr">
+      <c r="U17" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down. Remove plastic sleeve and replace carefully </t>
         </is>
       </c>
-      <c r="V17" s="105" t="inlineStr">
+      <c r="V17" s="4" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F06.04</t>
         </is>
       </c>
-      <c r="W17" s="109" t="n">
+      <c r="W17" s="15" t="n">
         <v>45511</v>
       </c>
-      <c r="X17" s="108" t="inlineStr">
+      <c r="X17" s="9" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y17" s="105" t="n"/>
-      <c r="Z17" s="110" t="inlineStr">
+      <c r="Y17" s="4" t="n"/>
+      <c r="Z17" s="6" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA17" s="105" t="inlineStr">
+      <c r="AA17" s="4" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB17" s="105" t="inlineStr">
+      <c r="AB17" s="4" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC17" s="105" t="n"/>
-      <c r="AD17" s="105" t="n"/>
-      <c r="AE17" s="105" t="n"/>
-      <c r="AF17" s="105" t="n"/>
-      <c r="AG17" s="105" t="n"/>
+      <c r="AC17" s="4" t="n"/>
+      <c r="AD17" s="4" t="n"/>
+      <c r="AE17" s="4" t="n"/>
+      <c r="AF17" s="4" t="n"/>
+      <c r="AG17" s="4" t="n"/>
     </row>
     <row r="18" ht="15.75" customHeight="1" s="5">
-      <c r="A18" s="103" t="inlineStr">
+      <c r="A18" s="1" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B18" s="104" t="n">
+      <c r="B18" s="11" t="n">
         <v>13300</v>
       </c>
-      <c r="C18" s="105" t="n"/>
-      <c r="D18" s="105" t="n"/>
-      <c r="E18" s="105" t="n"/>
-      <c r="F18" s="106" t="inlineStr">
+      <c r="C18" s="4" t="n"/>
+      <c r="D18" s="4" t="n"/>
+      <c r="E18" s="4" t="n"/>
+      <c r="F18" s="2" t="inlineStr">
         <is>
           <t>William Stanley biography, early transcript draft with manuscript inserts</t>
         </is>
       </c>
-      <c r="G18" s="105" t="n"/>
-      <c r="H18" s="106" t="inlineStr">
+      <c r="G18" s="4" t="n"/>
+      <c r="H18" s="2" t="inlineStr">
         <is>
           <t>Annotated Typescript Draft of "The Life of William Stanley" by Thomas C. Martin</t>
         </is>
       </c>
-      <c r="I18" s="105" t="inlineStr">
+      <c r="I18" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">Includes four drafts of Chapter 8. </t>
         </is>
       </c>
-      <c r="J18" s="103" t="inlineStr">
+      <c r="J18" s="1" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="K18" s="103" t="inlineStr">
+      <c r="K18" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L18" s="105" t="n"/>
-      <c r="M18" s="103" t="inlineStr">
+      <c r="L18" s="4" t="n"/>
+      <c r="M18" s="1" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N18" s="105" t="n"/>
-      <c r="O18" s="105" t="n"/>
-      <c r="P18" s="107" t="inlineStr">
+      <c r="N18" s="4" t="n"/>
+      <c r="O18" s="4" t="n"/>
+      <c r="P18" s="36" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q18" s="105" t="n"/>
-      <c r="R18" s="106" t="inlineStr">
+      <c r="Q18" s="4" t="n"/>
+      <c r="R18" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S18" s="108" t="inlineStr">
+      <c r="S18" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">154 pages </t>
         </is>
       </c>
-      <c r="T18" s="105" t="inlineStr">
+      <c r="T18" s="4" t="inlineStr">
         <is>
           <t>Box 8, Folder 6, Item 5</t>
         </is>
       </c>
-      <c r="U18" s="105" t="inlineStr">
+      <c r="U18" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down. Use caution to maintain orignal order. Some of the chapters are connected with plastic clips, please remove clips and do not replace them. </t>
         </is>
       </c>
-      <c r="V18" s="105" t="inlineStr">
+      <c r="V18" s="4" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F06.05</t>
         </is>
       </c>
-      <c r="W18" s="109" t="n">
+      <c r="W18" s="15" t="n">
         <v>45511</v>
       </c>
-      <c r="X18" s="108" t="inlineStr">
+      <c r="X18" s="9" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y18" s="105" t="n"/>
-      <c r="Z18" s="110" t="inlineStr">
+      <c r="Y18" s="4" t="n"/>
+      <c r="Z18" s="6" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA18" s="111" t="inlineStr">
+      <c r="AA18" s="13" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB18" s="105" t="inlineStr">
+      <c r="AB18" s="4" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC18" s="105" t="n"/>
-      <c r="AD18" s="105" t="n"/>
-      <c r="AE18" s="105" t="n"/>
-      <c r="AF18" s="105" t="n"/>
-      <c r="AG18" s="105" t="n"/>
+      <c r="AC18" s="4" t="n"/>
+      <c r="AD18" s="4" t="n"/>
+      <c r="AE18" s="4" t="n"/>
+      <c r="AF18" s="4" t="n"/>
+      <c r="AG18" s="4" t="n"/>
     </row>
     <row r="19" ht="15.75" customHeight="1" s="5">
-      <c r="A19" s="103" t="inlineStr">
+      <c r="A19" s="1" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B19" s="104" t="n">
+      <c r="B19" s="11" t="n">
         <v>13301</v>
       </c>
-      <c r="C19" s="105" t="n"/>
-      <c r="D19" s="105" t="n"/>
-      <c r="E19" s="105" t="n"/>
-      <c r="F19" s="106" t="inlineStr">
+      <c r="C19" s="4" t="n"/>
+      <c r="D19" s="4" t="n"/>
+      <c r="E19" s="4" t="n"/>
+      <c r="F19" s="2" t="inlineStr">
         <is>
           <t>William Stanley biography, printers typescript</t>
         </is>
       </c>
-      <c r="G19" s="105" t="n"/>
-      <c r="H19" s="106" t="inlineStr">
+      <c r="G19" s="4" t="n"/>
+      <c r="H19" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Printer's Typewritten Text of "The Life of William Stanley" by Thomas C. Martin with Handwritten Notes </t>
         </is>
       </c>
-      <c r="I19" s="105" t="n"/>
-      <c r="J19" s="103" t="inlineStr">
+      <c r="I19" s="4" t="n"/>
+      <c r="J19" s="1" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924</t>
         </is>
       </c>
-      <c r="K19" s="103" t="inlineStr">
+      <c r="K19" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L19" s="105" t="n"/>
-      <c r="M19" s="103" t="inlineStr">
+      <c r="L19" s="4" t="n"/>
+      <c r="M19" s="1" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N19" s="105" t="n"/>
-      <c r="O19" s="105" t="n"/>
-      <c r="P19" s="107" t="inlineStr">
+      <c r="N19" s="4" t="n"/>
+      <c r="O19" s="4" t="n"/>
+      <c r="P19" s="36" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q19" s="105" t="n"/>
-      <c r="R19" s="106" t="inlineStr">
+      <c r="Q19" s="4" t="n"/>
+      <c r="R19" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S19" s="108" t="inlineStr">
+      <c r="S19" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">99 pages </t>
         </is>
       </c>
-      <c r="T19" s="105" t="inlineStr">
+      <c r="T19" s="4" t="inlineStr">
         <is>
           <t>Box 8, Folder 7</t>
         </is>
       </c>
-      <c r="U19" s="105" t="inlineStr">
+      <c r="U19" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Up, Paper is Extremely Brittle </t>
         </is>
       </c>
-      <c r="V19" s="105" t="inlineStr">
+      <c r="V19" s="4" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F07</t>
         </is>
       </c>
-      <c r="W19" s="112" t="n">
+      <c r="W19" s="41" t="n">
         <v>45511</v>
       </c>
-      <c r="X19" s="108" t="inlineStr">
+      <c r="X19" s="9" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
-      <c r="Y19" s="105" t="n"/>
-      <c r="Z19" s="110" t="inlineStr">
+      <c r="Y19" s="4" t="n"/>
+      <c r="Z19" s="6" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA19" s="105" t="inlineStr">
+      <c r="AA19" s="4" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB19" s="105" t="inlineStr">
+      <c r="AB19" s="4" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC19" s="105" t="n"/>
-      <c r="AD19" s="105" t="n"/>
-      <c r="AE19" s="105" t="n"/>
-      <c r="AF19" s="105" t="n"/>
-      <c r="AG19" s="105" t="n"/>
+      <c r="AC19" s="4" t="n"/>
+      <c r="AD19" s="4" t="n"/>
+      <c r="AE19" s="4" t="n"/>
+      <c r="AF19" s="4" t="n"/>
+      <c r="AG19" s="4" t="n"/>
     </row>
     <row r="20" ht="15.75" customHeight="1" s="5">
-      <c r="A20" s="103" t="inlineStr">
+      <c r="A20" s="1" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B20" s="104" t="n">
+      <c r="B20" s="11" t="n">
         <v>13339</v>
       </c>
-      <c r="C20" s="105" t="n"/>
-      <c r="D20" s="105" t="n"/>
-      <c r="E20" s="105" t="n"/>
-      <c r="F20" s="106" t="inlineStr">
+      <c r="C20" s="4" t="n"/>
+      <c r="D20" s="4" t="n"/>
+      <c r="E20" s="4" t="n"/>
+      <c r="F20" s="2" t="inlineStr">
         <is>
           <t>"Associations with William Stanley," typescripts</t>
         </is>
       </c>
-      <c r="G20" s="105" t="n"/>
-      <c r="H20" s="106" t="inlineStr">
+      <c r="G20" s="4" t="n"/>
+      <c r="H20" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Typescript Draft of "Associates with William Stanley" by Cummings C. Chesney, Including "Play Ball" </t>
         </is>
       </c>
-      <c r="I20" s="105" t="n"/>
-      <c r="J20" s="103" t="inlineStr">
+      <c r="I20" s="4" t="n"/>
+      <c r="J20" s="1" t="inlineStr">
         <is>
           <t>Chesney, Cummings C.</t>
         </is>
       </c>
-      <c r="K20" s="103" t="inlineStr">
+      <c r="K20" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L20" s="105" t="n"/>
-      <c r="M20" s="103" t="inlineStr">
+      <c r="L20" s="4" t="n"/>
+      <c r="M20" s="1" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N20" s="105" t="n"/>
-      <c r="O20" s="105" t="n"/>
-      <c r="P20" s="107" t="inlineStr">
+      <c r="N20" s="4" t="n"/>
+      <c r="O20" s="4" t="n"/>
+      <c r="P20" s="36" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q20" s="105" t="n"/>
-      <c r="R20" s="106" t="inlineStr">
+      <c r="Q20" s="4" t="n"/>
+      <c r="R20" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S20" s="108" t="inlineStr">
+      <c r="S20" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">17 pages </t>
         </is>
       </c>
-      <c r="T20" s="105" t="inlineStr">
+      <c r="T20" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">Box 8, Folder 8, Item 1 </t>
         </is>
       </c>
-      <c r="U20" s="105" t="inlineStr">
+      <c r="U20" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down. </t>
         </is>
       </c>
-      <c r="V20" s="105" t="inlineStr">
+      <c r="V20" s="4" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F08.01</t>
         </is>
       </c>
-      <c r="W20" s="112" t="n">
+      <c r="W20" s="41" t="n">
         <v>45511</v>
       </c>
-      <c r="X20" s="105" t="inlineStr">
+      <c r="X20" s="4" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
-      <c r="Y20" s="105" t="n"/>
-      <c r="Z20" s="110" t="inlineStr">
+      <c r="Y20" s="4" t="n"/>
+      <c r="Z20" s="6" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA20" s="105" t="inlineStr">
+      <c r="AA20" s="4" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB20" s="105" t="inlineStr">
+      <c r="AB20" s="4" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC20" s="105" t="n"/>
-      <c r="AD20" s="105" t="n"/>
-      <c r="AE20" s="105" t="n"/>
-      <c r="AF20" s="105" t="n"/>
-      <c r="AG20" s="105" t="n"/>
+      <c r="AC20" s="4" t="n"/>
+      <c r="AD20" s="4" t="n"/>
+      <c r="AE20" s="4" t="n"/>
+      <c r="AF20" s="4" t="n"/>
+      <c r="AG20" s="4" t="n"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="5">
-      <c r="A21" s="103" t="inlineStr">
+      <c r="A21" s="1" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B21" s="104" t="n">
+      <c r="B21" s="11" t="n">
         <v>13339</v>
       </c>
-      <c r="C21" s="105" t="n"/>
-      <c r="D21" s="105" t="n"/>
-      <c r="E21" s="105" t="n"/>
-      <c r="F21" s="106" t="inlineStr">
+      <c r="C21" s="4" t="n"/>
+      <c r="D21" s="4" t="n"/>
+      <c r="E21" s="4" t="n"/>
+      <c r="F21" s="2" t="inlineStr">
         <is>
           <t>"Associations with William Stanley," typescripts</t>
         </is>
       </c>
-      <c r="G21" s="105" t="n"/>
-      <c r="H21" s="106" t="inlineStr">
+      <c r="G21" s="4" t="n"/>
+      <c r="H21" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Typescript Draft of "Associates with William Stanley" by Cummings C. Chesney, Untitled </t>
         </is>
       </c>
-      <c r="I21" s="105" t="n"/>
-      <c r="J21" s="103" t="inlineStr">
+      <c r="I21" s="4" t="n"/>
+      <c r="J21" s="1" t="inlineStr">
         <is>
           <t>Chesney, Cummings C.</t>
         </is>
       </c>
-      <c r="K21" s="103" t="inlineStr">
+      <c r="K21" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L21" s="105" t="n"/>
-      <c r="M21" s="103" t="inlineStr">
+      <c r="L21" s="4" t="n"/>
+      <c r="M21" s="1" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N21" s="105" t="n"/>
-      <c r="O21" s="105" t="n"/>
-      <c r="P21" s="107" t="inlineStr">
+      <c r="N21" s="4" t="n"/>
+      <c r="O21" s="4" t="n"/>
+      <c r="P21" s="36" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q21" s="105" t="n"/>
-      <c r="R21" s="106" t="inlineStr">
+      <c r="Q21" s="4" t="n"/>
+      <c r="R21" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S21" s="108" t="inlineStr">
+      <c r="S21" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">13 pages </t>
         </is>
       </c>
-      <c r="T21" s="105" t="inlineStr">
+      <c r="T21" s="4" t="inlineStr">
         <is>
           <t>Box 8, Folder 8, Item 2</t>
         </is>
       </c>
-      <c r="U21" s="105" t="inlineStr">
+      <c r="U21" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down. </t>
         </is>
       </c>
-      <c r="V21" s="105" t="inlineStr">
+      <c r="V21" s="4" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F08.02</t>
         </is>
       </c>
-      <c r="W21" s="109" t="n">
+      <c r="W21" s="15" t="n">
         <v>45511</v>
       </c>
-      <c r="X21" s="105" t="inlineStr">
+      <c r="X21" s="4" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
-      <c r="Y21" s="105" t="n"/>
-      <c r="Z21" s="110" t="inlineStr">
+      <c r="Y21" s="4" t="n"/>
+      <c r="Z21" s="6" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA21" s="105" t="inlineStr">
+      <c r="AA21" s="4" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB21" s="105" t="inlineStr">
+      <c r="AB21" s="4" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC21" s="105" t="n"/>
-      <c r="AD21" s="105" t="n"/>
-      <c r="AE21" s="105" t="n"/>
-      <c r="AF21" s="105" t="n"/>
-      <c r="AG21" s="105" t="n"/>
+      <c r="AC21" s="4" t="n"/>
+      <c r="AD21" s="4" t="n"/>
+      <c r="AE21" s="4" t="n"/>
+      <c r="AF21" s="4" t="n"/>
+      <c r="AG21" s="4" t="n"/>
     </row>
     <row r="22" ht="15.75" customHeight="1" s="5">
-      <c r="A22" s="103" t="inlineStr">
+      <c r="A22" s="1" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B22" s="104" t="n">
+      <c r="B22" s="11" t="n">
         <v>13339</v>
       </c>
-      <c r="C22" s="105" t="n"/>
-      <c r="D22" s="105" t="n"/>
-      <c r="E22" s="105" t="n"/>
-      <c r="F22" s="106" t="inlineStr">
+      <c r="C22" s="4" t="n"/>
+      <c r="D22" s="4" t="n"/>
+      <c r="E22" s="4" t="n"/>
+      <c r="F22" s="2" t="inlineStr">
         <is>
           <t>"Associations with William Stanley," typescripts</t>
         </is>
       </c>
-      <c r="G22" s="105" t="n"/>
-      <c r="H22" s="106" t="inlineStr">
+      <c r="G22" s="4" t="n"/>
+      <c r="H22" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Typescript Draft of "Associates with William Stanley" by Cummings C. Chesney, Untitled from Scientific and Industrial Information Bureau </t>
         </is>
       </c>
-      <c r="I22" s="105" t="n"/>
-      <c r="J22" s="103" t="inlineStr">
+      <c r="I22" s="4" t="n"/>
+      <c r="J22" s="1" t="inlineStr">
         <is>
           <t>Chesney, Cummings C.</t>
         </is>
       </c>
-      <c r="K22" s="103" t="inlineStr">
+      <c r="K22" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Author </t>
         </is>
       </c>
-      <c r="L22" s="105" t="n"/>
-      <c r="M22" s="103" t="inlineStr">
+      <c r="L22" s="4" t="n"/>
+      <c r="M22" s="1" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="N22" s="105" t="n"/>
-      <c r="O22" s="105" t="n"/>
-      <c r="P22" s="107" t="inlineStr">
+      <c r="N22" s="4" t="n"/>
+      <c r="O22" s="4" t="n"/>
+      <c r="P22" s="36" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="Q22" s="105" t="n"/>
-      <c r="R22" s="106" t="inlineStr">
+      <c r="Q22" s="4" t="n"/>
+      <c r="R22" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S22" s="108" t="inlineStr">
+      <c r="S22" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">30 pages </t>
         </is>
       </c>
-      <c r="T22" s="105" t="inlineStr">
+      <c r="T22" s="4" t="inlineStr">
         <is>
           <t>Box 8, Folder 8, Item 3</t>
         </is>
       </c>
-      <c r="U22" s="105" t="inlineStr">
+      <c r="U22" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down. </t>
         </is>
       </c>
-      <c r="V22" s="105" t="inlineStr">
+      <c r="V22" s="4" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B08.F08.03</t>
         </is>
       </c>
-      <c r="W22" s="109" t="n">
+      <c r="W22" s="15" t="n">
         <v>45511</v>
       </c>
-      <c r="X22" s="105" t="inlineStr">
+      <c r="X22" s="4" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
-      <c r="Y22" s="105" t="n"/>
-      <c r="Z22" s="110" t="inlineStr">
+      <c r="Y22" s="4" t="n"/>
+      <c r="Z22" s="6" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AA22" s="105" t="inlineStr">
+      <c r="AA22" s="4" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AB22" s="105" t="inlineStr">
+      <c r="AB22" s="4" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AC22" s="105" t="n"/>
-      <c r="AD22" s="105" t="n"/>
-      <c r="AE22" s="105" t="n"/>
-      <c r="AF22" s="105" t="n"/>
-      <c r="AG22" s="105" t="n"/>
+      <c r="AC22" s="4" t="n"/>
+      <c r="AD22" s="4" t="n"/>
+      <c r="AE22" s="4" t="n"/>
+      <c r="AF22" s="4" t="n"/>
+      <c r="AG22" s="4" t="n"/>
     </row>
     <row r="23" ht="12.75" customHeight="1" s="5">
       <c r="P23" s="38" t="n"/>
@@ -18083,105 +18083,90 @@
       </c>
     </row>
     <row r="136" ht="15" customHeight="1" s="5">
-      <c r="A136" s="110" t="inlineStr">
+      <c r="A136" s="6" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B136" s="113" t="n">
+      <c r="B136" s="7" t="n">
         <v>13344</v>
       </c>
-      <c r="C136" s="110" t="n"/>
-      <c r="D136" s="110" t="n"/>
-      <c r="E136" s="110" t="n"/>
-      <c r="F136" s="110" t="inlineStr">
+      <c r="C136" s="6" t="n"/>
+      <c r="D136" s="6" t="n"/>
+      <c r="E136" s="6" t="n"/>
+      <c r="F136" s="6" t="inlineStr">
         <is>
           <t>Correspondence regarding William Stanley biography</t>
         </is>
       </c>
-      <c r="G136" s="114" t="n"/>
-      <c r="H136" s="108" t="inlineStr">
+      <c r="H136" s="9" t="inlineStr">
         <is>
           <t>Letter from C. C. Chesney to T. C. Martin, November 13, 1922, with enclosures</t>
         </is>
       </c>
-      <c r="I136" s="108" t="inlineStr">
+      <c r="I136" s="9" t="inlineStr">
         <is>
           <t>Enclosures: Letter from F. Darlington to T. C. Martin, November 5, 1922 and letter from  Philip G. Gossler to T. C. Martin, November 6, 1922</t>
         </is>
       </c>
-      <c r="J136" s="108" t="inlineStr">
+      <c r="J136" s="9" t="inlineStr">
         <is>
           <t>Chesney, Cummings C.;Darlington, Frederick;Gossler, Philip G.</t>
         </is>
       </c>
-      <c r="K136" s="114" t="n"/>
-      <c r="L136" s="114" t="n"/>
-      <c r="M136" s="114" t="n"/>
-      <c r="N136" s="108" t="inlineStr">
+      <c r="N136" s="9" t="inlineStr">
         <is>
           <t>Martin, Thomas Commerford, 1856-1924;Stanley, William, 1858-1916</t>
         </is>
       </c>
-      <c r="O136" s="114" t="n"/>
-      <c r="P136" s="114" t="n"/>
-      <c r="Q136" s="115" t="inlineStr">
+      <c r="Q136" s="40" t="inlineStr">
         <is>
           <t>1922-11-06;1922-11-08;1922-11-13</t>
         </is>
       </c>
-      <c r="R136" s="114" t="n"/>
-      <c r="S136" s="108" t="inlineStr">
+      <c r="S136" s="9" t="inlineStr">
         <is>
           <t>No Copyright - United States</t>
         </is>
       </c>
-      <c r="T136" s="114" t="n"/>
-      <c r="U136" s="110" t="inlineStr">
+      <c r="U136" s="6" t="inlineStr">
         <is>
           <t>Box 9, Folder 5, Item 81</t>
         </is>
       </c>
-      <c r="V136" s="116" t="inlineStr">
+      <c r="V136" s="8" t="inlineStr">
         <is>
           <t>Glass down</t>
         </is>
       </c>
-      <c r="W136" s="108" t="inlineStr">
+      <c r="W136" s="9" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B09.F05.81</t>
         </is>
       </c>
-      <c r="X136" s="117" t="n">
+      <c r="X136" s="16" t="n">
         <v>45523</v>
       </c>
-      <c r="Y136" s="108" t="inlineStr">
+      <c r="Y136" s="9" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Z136" s="114" t="n"/>
-      <c r="AA136" s="110" t="inlineStr">
+      <c r="AA136" s="6" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AB136" s="114" t="inlineStr">
+      <c r="AB136" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AC136" s="114" t="inlineStr">
+      <c r="AC136" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AD136" s="114" t="n"/>
-      <c r="AE136" s="114" t="n"/>
-      <c r="AF136" s="114" t="n"/>
-      <c r="AG136" s="114" t="n"/>
-      <c r="AH136" s="114" t="n"/>
-      <c r="AI136" s="114" t="n"/>
     </row>
     <row r="137" ht="15" customHeight="1" s="5">
       <c r="A137" s="6" t="inlineStr">
@@ -23039,101 +23024,85 @@
       </c>
     </row>
     <row r="198" ht="15" customHeight="1" s="5">
-      <c r="A198" s="110" t="inlineStr">
+      <c r="A198" s="6" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B198" s="113" t="n">
+      <c r="B198" s="7" t="n">
         <v>13346</v>
       </c>
-      <c r="C198" s="110" t="n"/>
-      <c r="D198" s="110" t="n"/>
-      <c r="E198" s="110" t="n"/>
-      <c r="F198" s="110" t="inlineStr">
+      <c r="C198" s="6" t="n"/>
+      <c r="D198" s="6" t="n"/>
+      <c r="E198" s="6" t="n"/>
+      <c r="F198" s="6" t="inlineStr">
         <is>
           <t>Biographical articles and brochures</t>
         </is>
       </c>
-      <c r="G198" s="114" t="n"/>
-      <c r="H198" s="110" t="inlineStr">
+      <c r="H198" s="6" t="inlineStr">
         <is>
           <t>Biographical articles and brochures, Item 9</t>
         </is>
       </c>
-      <c r="I198" s="114" t="n"/>
-      <c r="J198" s="108" t="inlineStr">
+      <c r="J198" s="9" t="inlineStr">
         <is>
           <t>unknown</t>
         </is>
       </c>
-      <c r="K198" s="114" t="n"/>
-      <c r="L198" s="114" t="n"/>
-      <c r="M198" s="114" t="n"/>
-      <c r="N198" s="108" t="inlineStr">
+      <c r="N198" s="9" t="inlineStr">
         <is>
           <t>Stanley, William, 1858-1916</t>
         </is>
       </c>
-      <c r="O198" s="114" t="n"/>
-      <c r="P198" s="114" t="n"/>
-      <c r="Q198" s="115" t="inlineStr">
+      <c r="Q198" s="40" t="inlineStr">
         <is>
           <t>unknown</t>
         </is>
       </c>
-      <c r="R198" s="114" t="n"/>
-      <c r="S198" s="108" t="inlineStr">
+      <c r="S198" s="9" t="inlineStr">
         <is>
           <t>Copyright Undetermined</t>
         </is>
       </c>
-      <c r="T198" s="114" t="n"/>
-      <c r="U198" s="108" t="inlineStr">
+      <c r="U198" s="9" t="inlineStr">
         <is>
           <t>Box 9, Folder 8, Item 9</t>
         </is>
       </c>
-      <c r="V198" s="116" t="inlineStr">
+      <c r="V198" s="8" t="inlineStr">
         <is>
           <t>Glass down</t>
         </is>
       </c>
-      <c r="W198" s="108" t="inlineStr">
+      <c r="W198" s="9" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B09.F08.09</t>
         </is>
       </c>
-      <c r="X198" s="117" t="n">
+      <c r="X198" s="16" t="n">
         <v>45524</v>
       </c>
-      <c r="Y198" s="108" t="inlineStr">
+      <c r="Y198" s="9" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Z198" s="114" t="n"/>
-      <c r="AA198" s="110" t="inlineStr">
+      <c r="AA198" s="6" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="AB198" s="114" t="inlineStr">
+      <c r="AB198" t="inlineStr">
         <is>
           <t>AUTO</t>
         </is>
       </c>
-      <c r="AC198" s="114" t="inlineStr">
+      <c r="AC198" t="inlineStr">
         <is>
           <t>File does not exist</t>
         </is>
       </c>
-      <c r="AD198" s="114" t="n"/>
-      <c r="AE198" s="114" t="n"/>
-      <c r="AF198" s="114" t="n"/>
-      <c r="AG198" s="114" t="n"/>
-      <c r="AH198" s="114" t="n"/>
-      <c r="AI198" s="114" t="n"/>
     </row>
     <row r="199" ht="15" customHeight="1" s="5">
       <c r="A199" s="6" t="inlineStr">

</xml_diff>